<commit_message>
Updates as of 7/11/2020
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris_hoover\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035796DF-6140-C942-8FFC-A1DB34B61927}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4160" yWindow="720" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{50240998-A895-7F42-B834-945925070EED}"/>
+    <workbookView xWindow="4155" yWindow="720" windowWidth="29445" windowHeight="19500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters with Distributions" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
     <sheet name="PUI Details" sheetId="7" r:id="rId5"/>
     <sheet name="Internal" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -287,7 +286,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -884,22 +883,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF7E970-76F8-6942-B4A0-7B2C1D2884B8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" style="30" customWidth="1"/>
     <col min="2" max="2" width="62.5" style="2" customWidth="1"/>
-    <col min="3" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="1"/>
+    <col min="3" max="4" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>12</v>
       </c>
@@ -913,7 +912,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>73</v>
       </c>
@@ -927,7 +926,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>74</v>
       </c>
@@ -941,7 +940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>45</v>
       </c>
@@ -955,7 +954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>46</v>
       </c>
@@ -969,7 +968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>47</v>
       </c>
@@ -983,7 +982,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>48</v>
       </c>
@@ -997,7 +996,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>44</v>
       </c>
@@ -1011,7 +1010,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>51</v>
       </c>
@@ -1025,7 +1024,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>52</v>
       </c>
@@ -1041,11 +1040,11 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D2" xr:uid="{39F8344C-73C3-994E-96EF-A9BFB1D45FA6}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D2">
       <formula1>0</formula1>
       <formula2>20</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:D10" xr:uid="{9F0C0177-DE3E-1444-856B-A1A4910CD57E}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:D10">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -1055,21 +1054,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5372A5C3-523B-5F40-A7DB-9F78D72AADAB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.375" customWidth="1"/>
+    <col min="4" max="4" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>57</v>
       </c>
@@ -1083,7 +1082,7 @@
       </c>
       <c r="F1" s="38"/>
     </row>
-    <row r="2" spans="1:6" s="28" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="28" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>35</v>
       </c>
@@ -1103,7 +1102,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>67</v>
       </c>
@@ -1123,7 +1122,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>43897</v>
       </c>
@@ -1143,7 +1142,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>43907</v>
       </c>
@@ -1163,7 +1162,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>43927</v>
       </c>
@@ -1183,7 +1182,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>43941</v>
       </c>
@@ -1203,7 +1202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>43955</v>
       </c>
@@ -1223,7 +1222,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>43969</v>
       </c>
@@ -1243,7 +1242,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>43983</v>
       </c>
@@ -1263,7 +1262,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>43997</v>
       </c>
@@ -1290,11 +1289,11 @@
     <mergeCell ref="E1:F1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A11" xr:uid="{55857FF0-8ABD-E94F-8530-47F7128019AC}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A11">
       <formula1>43831</formula1>
       <formula2>44196</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{9B674EB0-0B81-E446-AFB3-06ADC0DD22FE}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
       <formula1>0</formula1>
       <formula2>30</formula2>
     </dataValidation>
@@ -1304,20 +1303,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BCB5455-61A0-9A48-A110-20902745EBF4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="22.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
@@ -1328,7 +1327,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -1339,7 +1338,7 @@
         <v>883305</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>21</v>
       </c>
@@ -1350,7 +1349,7 @@
         <v>43905</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
@@ -1363,11 +1362,11 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{88106E44-DD25-724E-9428-A2C12A1073F6}">
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="C2">
       <formula1>0</formula1>
       <formula2>100000000</formula2>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C4" xr:uid="{E9B6D3E5-D408-1D41-9CF1-E5EA3191C411}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C4">
       <formula1>43831</formula1>
       <formula2>44561</formula2>
     </dataValidation>
@@ -1377,28 +1376,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9816A416-5B6A-4545-98DF-6AED7BBC6987}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I305"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="20" topLeftCell="G91" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="20" topLeftCell="G112" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="F113" sqref="F113"/>
+      <selection pane="bottomRight" activeCell="F114" sqref="F114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.5" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" style="3" customWidth="1"/>
-    <col min="4" max="7" width="12.83203125" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.125" style="3" customWidth="1"/>
+    <col min="4" max="7" width="12.875" customWidth="1"/>
+    <col min="8" max="8" width="12.875" style="3" customWidth="1"/>
     <col min="9" max="9" width="14.5" style="3" customWidth="1"/>
     <col min="10" max="10" width="45.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="16"/>
       <c r="B1" s="42" t="s">
         <v>25</v>
@@ -1417,7 +1416,7 @@
       </c>
       <c r="I1" s="39"/>
     </row>
-    <row r="2" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="41" t="s">
         <v>29</v>
       </c>
@@ -1435,7 +1434,7 @@
       </c>
       <c r="I2" s="40"/>
     </row>
-    <row r="3" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>5</v>
       </c>
@@ -1464,7 +1463,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>28</v>
       </c>
@@ -1493,7 +1492,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
         <v>43913</v>
       </c>
@@ -1516,7 +1515,7 @@
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="18">
         <v>43914</v>
       </c>
@@ -1539,7 +1538,7 @@
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="18">
         <v>43915</v>
       </c>
@@ -1562,7 +1561,7 @@
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="18">
         <v>43916</v>
       </c>
@@ -1585,7 +1584,7 @@
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="18">
         <v>43917</v>
       </c>
@@ -1608,7 +1607,7 @@
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="18">
         <v>43918</v>
       </c>
@@ -1631,7 +1630,7 @@
       <c r="H10" s="19"/>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
         <v>43919</v>
       </c>
@@ -1654,7 +1653,7 @@
       <c r="H11" s="23"/>
       <c r="I11" s="19"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="18">
         <v>43920</v>
       </c>
@@ -1677,7 +1676,7 @@
       <c r="H12" s="23"/>
       <c r="I12" s="19"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="18">
         <v>43921</v>
       </c>
@@ -1700,7 +1699,7 @@
       <c r="H13" s="23"/>
       <c r="I13" s="19"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="18">
         <v>43922</v>
       </c>
@@ -1723,7 +1722,7 @@
       <c r="H14" s="23"/>
       <c r="I14" s="19"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="18">
         <v>43923</v>
       </c>
@@ -1746,7 +1745,7 @@
       <c r="H15" s="23"/>
       <c r="I15" s="19"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="18">
         <v>43924</v>
       </c>
@@ -1769,7 +1768,7 @@
       <c r="H16" s="23"/>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="18">
         <v>43925</v>
       </c>
@@ -1792,7 +1791,7 @@
       <c r="H17" s="23"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="18">
         <v>43926</v>
       </c>
@@ -1815,7 +1814,7 @@
       <c r="H18" s="23"/>
       <c r="I18" s="19"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="18">
         <v>43927</v>
       </c>
@@ -1838,7 +1837,7 @@
       <c r="H19" s="23"/>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="20">
         <v>43928</v>
       </c>
@@ -1861,7 +1860,7 @@
       <c r="H20" s="23"/>
       <c r="I20" s="19"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="20">
         <v>43929</v>
       </c>
@@ -1884,7 +1883,7 @@
       <c r="H21" s="23"/>
       <c r="I21" s="19"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <v>43930</v>
       </c>
@@ -1907,7 +1906,7 @@
       <c r="H22" s="23"/>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="20">
         <v>43931</v>
       </c>
@@ -1930,7 +1929,7 @@
       <c r="H23" s="23"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="20">
         <v>43932</v>
       </c>
@@ -1953,7 +1952,7 @@
       <c r="H24" s="23"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
         <v>43933</v>
       </c>
@@ -1976,7 +1975,7 @@
       <c r="H25" s="23"/>
       <c r="I25" s="19"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
         <v>43934</v>
       </c>
@@ -1999,7 +1998,7 @@
       <c r="H26" s="23"/>
       <c r="I26" s="19"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="20">
         <v>43935</v>
       </c>
@@ -2022,7 +2021,7 @@
       <c r="H27" s="23"/>
       <c r="I27" s="19"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="20">
         <v>43936</v>
       </c>
@@ -2045,7 +2044,7 @@
       <c r="H28" s="23"/>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="20">
         <v>43937</v>
       </c>
@@ -2068,7 +2067,7 @@
       <c r="H29" s="23"/>
       <c r="I29" s="19"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="20">
         <v>43938</v>
       </c>
@@ -2091,7 +2090,7 @@
       <c r="H30" s="23"/>
       <c r="I30" s="19"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="20">
         <v>43939</v>
       </c>
@@ -2114,7 +2113,7 @@
       <c r="H31" s="23"/>
       <c r="I31" s="19"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="20">
         <v>43940</v>
       </c>
@@ -2137,7 +2136,7 @@
       <c r="H32" s="23"/>
       <c r="I32" s="19"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="20">
         <v>43941</v>
       </c>
@@ -2160,7 +2159,7 @@
       <c r="H33" s="23"/>
       <c r="I33" s="19"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="20">
         <v>43942</v>
       </c>
@@ -2183,7 +2182,7 @@
       <c r="H34" s="23"/>
       <c r="I34" s="19"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="20">
         <v>43943</v>
       </c>
@@ -2206,7 +2205,7 @@
       <c r="H35" s="23"/>
       <c r="I35" s="19"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="20">
         <v>43944</v>
       </c>
@@ -2229,7 +2228,7 @@
       <c r="H36" s="23"/>
       <c r="I36" s="19"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="20">
         <v>43945</v>
       </c>
@@ -2252,7 +2251,7 @@
       <c r="H37" s="23"/>
       <c r="I37" s="19"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="20">
         <v>43946</v>
       </c>
@@ -2275,7 +2274,7 @@
       <c r="H38" s="23"/>
       <c r="I38" s="19"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="20">
         <v>43947</v>
       </c>
@@ -2298,7 +2297,7 @@
       <c r="H39" s="23"/>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="20">
         <v>43948</v>
       </c>
@@ -2321,7 +2320,7 @@
       <c r="H40" s="23"/>
       <c r="I40" s="19"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="20">
         <v>43949</v>
       </c>
@@ -2344,7 +2343,7 @@
       <c r="H41" s="23"/>
       <c r="I41" s="19"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="20">
         <v>43950</v>
       </c>
@@ -2367,7 +2366,7 @@
       <c r="H42" s="23"/>
       <c r="I42" s="19"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="20">
         <v>43951</v>
       </c>
@@ -2390,7 +2389,7 @@
       <c r="H43" s="23"/>
       <c r="I43" s="19"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="20">
         <v>43952</v>
       </c>
@@ -2413,7 +2412,7 @@
       <c r="H44" s="23"/>
       <c r="I44" s="19"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="20">
         <v>43953</v>
       </c>
@@ -2436,7 +2435,7 @@
       <c r="H45" s="23"/>
       <c r="I45" s="19"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="20">
         <v>43954</v>
       </c>
@@ -2459,7 +2458,7 @@
       <c r="H46" s="23"/>
       <c r="I46" s="19"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="20">
         <v>43955</v>
       </c>
@@ -2482,7 +2481,7 @@
       <c r="H47" s="23"/>
       <c r="I47" s="19"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="20">
         <v>43956</v>
       </c>
@@ -2505,7 +2504,7 @@
       <c r="H48" s="23"/>
       <c r="I48" s="19"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="20">
         <v>43957</v>
       </c>
@@ -2528,7 +2527,7 @@
       <c r="H49" s="23"/>
       <c r="I49" s="19"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="20">
         <v>43958</v>
       </c>
@@ -2551,7 +2550,7 @@
       <c r="H50" s="23"/>
       <c r="I50" s="19"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="20">
         <v>43959</v>
       </c>
@@ -2574,7 +2573,7 @@
       <c r="H51" s="23"/>
       <c r="I51" s="19"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="20">
         <v>43960</v>
       </c>
@@ -2597,7 +2596,7 @@
       <c r="H52" s="23"/>
       <c r="I52" s="19"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="20">
         <v>43961</v>
       </c>
@@ -2620,7 +2619,7 @@
       <c r="H53" s="23"/>
       <c r="I53" s="19"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="20">
         <v>43962</v>
       </c>
@@ -2643,7 +2642,7 @@
       <c r="H54" s="23"/>
       <c r="I54" s="19"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="20">
         <v>43963</v>
       </c>
@@ -2666,7 +2665,7 @@
       <c r="H55" s="23"/>
       <c r="I55" s="19"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="20">
         <v>43964</v>
       </c>
@@ -2689,7 +2688,7 @@
       <c r="H56" s="23"/>
       <c r="I56" s="19"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="20">
         <v>43965</v>
       </c>
@@ -2712,7 +2711,7 @@
       <c r="H57" s="23"/>
       <c r="I57" s="19"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="20">
         <v>43966</v>
       </c>
@@ -2735,7 +2734,7 @@
       <c r="H58" s="23"/>
       <c r="I58" s="19"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="20">
         <v>43967</v>
       </c>
@@ -2758,7 +2757,7 @@
       <c r="H59" s="23"/>
       <c r="I59" s="19"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="20">
         <v>43968</v>
       </c>
@@ -2781,7 +2780,7 @@
       <c r="H60" s="23"/>
       <c r="I60" s="19"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="20">
         <v>43969</v>
       </c>
@@ -2804,7 +2803,7 @@
       <c r="H61" s="23"/>
       <c r="I61" s="19"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="20">
         <v>43970</v>
       </c>
@@ -2827,7 +2826,7 @@
       <c r="H62" s="23"/>
       <c r="I62" s="19"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="20">
         <v>43971</v>
       </c>
@@ -2850,7 +2849,7 @@
       <c r="H63" s="23"/>
       <c r="I63" s="19"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="20">
         <v>43972</v>
       </c>
@@ -2873,7 +2872,7 @@
       <c r="H64" s="23"/>
       <c r="I64" s="19"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="24">
         <v>43973</v>
       </c>
@@ -2896,7 +2895,7 @@
       <c r="H65" s="23"/>
       <c r="I65" s="19"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="24">
         <v>43974</v>
       </c>
@@ -2919,7 +2918,7 @@
       <c r="H66" s="19"/>
       <c r="I66" s="19"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="24">
         <v>43975</v>
       </c>
@@ -2942,7 +2941,7 @@
       <c r="H67" s="19"/>
       <c r="I67" s="19"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="24">
         <v>43976</v>
       </c>
@@ -2965,7 +2964,7 @@
       <c r="H68" s="19"/>
       <c r="I68" s="19"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="24">
         <v>43977</v>
       </c>
@@ -2988,7 +2987,7 @@
       <c r="H69" s="19"/>
       <c r="I69" s="19"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="24">
         <v>43978</v>
       </c>
@@ -3011,7 +3010,7 @@
       <c r="H70" s="19"/>
       <c r="I70" s="19"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="20">
         <v>43979</v>
       </c>
@@ -3034,7 +3033,7 @@
       <c r="H71" s="19"/>
       <c r="I71" s="19"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="20">
         <v>43980</v>
       </c>
@@ -3057,7 +3056,7 @@
       <c r="H72" s="19"/>
       <c r="I72" s="19"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="20">
         <v>43981</v>
       </c>
@@ -3080,7 +3079,7 @@
       <c r="H73" s="19"/>
       <c r="I73" s="19"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="20">
         <v>43982</v>
       </c>
@@ -3103,7 +3102,7 @@
       <c r="H74" s="19"/>
       <c r="I74" s="19"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="20">
         <v>43983</v>
       </c>
@@ -3126,7 +3125,7 @@
       <c r="H75" s="19"/>
       <c r="I75" s="19"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="20">
         <v>43984</v>
       </c>
@@ -3149,7 +3148,7 @@
       <c r="H76" s="19"/>
       <c r="I76" s="19"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="20">
         <v>43985</v>
       </c>
@@ -3172,7 +3171,7 @@
       <c r="H77" s="19"/>
       <c r="I77" s="19"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="20">
         <v>43986</v>
       </c>
@@ -3195,7 +3194,7 @@
       <c r="H78" s="19"/>
       <c r="I78" s="19"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="20">
         <v>43987</v>
       </c>
@@ -3218,7 +3217,7 @@
       <c r="H79" s="19"/>
       <c r="I79" s="19"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="20">
         <v>43988</v>
       </c>
@@ -3241,7 +3240,7 @@
       <c r="H80" s="19"/>
       <c r="I80" s="19"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="20">
         <v>43989</v>
       </c>
@@ -3264,7 +3263,7 @@
       <c r="H81" s="19"/>
       <c r="I81" s="19"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="20">
         <v>43990</v>
       </c>
@@ -3287,7 +3286,7 @@
       <c r="H82" s="19"/>
       <c r="I82" s="19"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="20">
         <v>43991</v>
       </c>
@@ -3310,7 +3309,7 @@
       <c r="H83" s="19"/>
       <c r="I83" s="19"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="20">
         <v>43992</v>
       </c>
@@ -3333,7 +3332,7 @@
       <c r="H84" s="19"/>
       <c r="I84" s="19"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="20">
         <v>43993</v>
       </c>
@@ -3356,7 +3355,7 @@
       <c r="H85" s="19"/>
       <c r="I85" s="19"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="20">
         <v>43994</v>
       </c>
@@ -3379,7 +3378,7 @@
       <c r="H86" s="19"/>
       <c r="I86" s="19"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="20">
         <v>43995</v>
       </c>
@@ -3402,7 +3401,7 @@
       <c r="H87" s="19"/>
       <c r="I87" s="19"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="20">
         <v>43996</v>
       </c>
@@ -3425,7 +3424,7 @@
       <c r="H88" s="19"/>
       <c r="I88" s="19"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="20">
         <v>43997</v>
       </c>
@@ -3448,7 +3447,7 @@
       <c r="H89" s="19"/>
       <c r="I89" s="19"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="20">
         <v>43998</v>
       </c>
@@ -3471,7 +3470,7 @@
       <c r="H90" s="19"/>
       <c r="I90" s="19"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="20">
         <v>43999</v>
       </c>
@@ -3494,7 +3493,7 @@
       <c r="H91" s="19"/>
       <c r="I91" s="19"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="20">
         <v>44000</v>
       </c>
@@ -3517,7 +3516,7 @@
       <c r="H92" s="19"/>
       <c r="I92" s="19"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="20">
         <v>44001</v>
       </c>
@@ -3540,7 +3539,7 @@
       <c r="H93" s="19"/>
       <c r="I93" s="19"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="20">
         <v>44002</v>
       </c>
@@ -3563,7 +3562,7 @@
       <c r="H94" s="19"/>
       <c r="I94" s="19"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="20">
         <v>44003</v>
       </c>
@@ -3586,7 +3585,7 @@
       <c r="H95" s="19"/>
       <c r="I95" s="19"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="20">
         <v>44004</v>
       </c>
@@ -3609,7 +3608,7 @@
       <c r="H96" s="19"/>
       <c r="I96" s="19"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="20">
         <v>44005</v>
       </c>
@@ -3632,7 +3631,7 @@
       <c r="H97" s="19"/>
       <c r="I97" s="19"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="20">
         <v>44006</v>
       </c>
@@ -3655,7 +3654,7 @@
       <c r="H98" s="19"/>
       <c r="I98" s="19"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="20">
         <v>44007</v>
       </c>
@@ -3678,7 +3677,7 @@
       <c r="H99" s="19"/>
       <c r="I99" s="19"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="20">
         <v>44008</v>
       </c>
@@ -3701,7 +3700,7 @@
       <c r="H100" s="19"/>
       <c r="I100" s="19"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="20">
         <v>44009</v>
       </c>
@@ -3724,7 +3723,7 @@
       <c r="H101" s="19"/>
       <c r="I101" s="19"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="20">
         <v>44010</v>
       </c>
@@ -3747,7 +3746,7 @@
       <c r="H102" s="19"/>
       <c r="I102" s="19"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="20">
         <v>44011</v>
       </c>
@@ -3770,7 +3769,7 @@
       <c r="H103" s="19"/>
       <c r="I103" s="19"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="20">
         <v>44012</v>
       </c>
@@ -3793,7 +3792,7 @@
       <c r="H104" s="19"/>
       <c r="I104" s="19"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="20">
         <v>44013</v>
       </c>
@@ -3816,7 +3815,7 @@
       <c r="H105" s="19"/>
       <c r="I105" s="19"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="20">
         <v>44014</v>
       </c>
@@ -3839,7 +3838,7 @@
       <c r="H106" s="19"/>
       <c r="I106" s="19"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="20">
         <v>44015</v>
       </c>
@@ -3862,7 +3861,7 @@
       <c r="H107" s="19"/>
       <c r="I107" s="19"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="20">
         <v>44016</v>
       </c>
@@ -3885,7 +3884,7 @@
       <c r="H108" s="19"/>
       <c r="I108" s="19"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="20">
         <v>44017</v>
       </c>
@@ -3908,7 +3907,7 @@
       <c r="H109" s="19"/>
       <c r="I109" s="19"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="20">
         <v>44018</v>
       </c>
@@ -3931,7 +3930,7 @@
       <c r="H110" s="19"/>
       <c r="I110" s="19"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="20">
         <v>44019</v>
       </c>
@@ -3954,7 +3953,7 @@
       <c r="H111" s="19"/>
       <c r="I111" s="19"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="20">
         <v>44020</v>
       </c>
@@ -3977,18 +3976,30 @@
       <c r="H112" s="19"/>
       <c r="I112" s="19"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A113" s="20"/>
-      <c r="B113" s="19"/>
-      <c r="C113" s="19"/>
-      <c r="D113" s="23"/>
-      <c r="E113" s="23"/>
-      <c r="F113" s="23"/>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" s="20">
+        <v>44021</v>
+      </c>
+      <c r="B113" s="19">
+        <v>59</v>
+      </c>
+      <c r="C113" s="19">
+        <v>24</v>
+      </c>
+      <c r="D113" s="23">
+        <v>19</v>
+      </c>
+      <c r="E113" s="23">
+        <v>1</v>
+      </c>
+      <c r="F113" s="23">
+        <v>50</v>
+      </c>
       <c r="G113" s="23"/>
       <c r="H113" s="19"/>
       <c r="I113" s="19"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="20"/>
       <c r="B114" s="19"/>
       <c r="C114" s="19"/>
@@ -3999,7 +4010,7 @@
       <c r="H114" s="19"/>
       <c r="I114" s="19"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="20"/>
       <c r="B115" s="19"/>
       <c r="C115" s="19"/>
@@ -4010,7 +4021,7 @@
       <c r="H115" s="19"/>
       <c r="I115" s="19"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="20"/>
       <c r="B116" s="19"/>
       <c r="C116" s="19"/>
@@ -4021,7 +4032,7 @@
       <c r="H116" s="19"/>
       <c r="I116" s="19"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="20"/>
       <c r="B117" s="19"/>
       <c r="C117" s="19"/>
@@ -4032,7 +4043,7 @@
       <c r="H117" s="19"/>
       <c r="I117" s="19"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="20"/>
       <c r="B118" s="19"/>
       <c r="C118" s="19"/>
@@ -4043,7 +4054,7 @@
       <c r="H118" s="19"/>
       <c r="I118" s="19"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="20"/>
       <c r="B119" s="19"/>
       <c r="C119" s="19"/>
@@ -4054,7 +4065,7 @@
       <c r="H119" s="19"/>
       <c r="I119" s="19"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="20"/>
       <c r="B120" s="19"/>
       <c r="C120" s="19"/>
@@ -4065,7 +4076,7 @@
       <c r="H120" s="19"/>
       <c r="I120" s="19"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="20"/>
       <c r="B121" s="19"/>
       <c r="C121" s="19"/>
@@ -4076,7 +4087,7 @@
       <c r="H121" s="19"/>
       <c r="I121" s="19"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="20"/>
       <c r="B122" s="19"/>
       <c r="C122" s="19"/>
@@ -4087,7 +4098,7 @@
       <c r="H122" s="19"/>
       <c r="I122" s="19"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="20"/>
       <c r="B123" s="19"/>
       <c r="C123" s="19"/>
@@ -4098,7 +4109,7 @@
       <c r="H123" s="19"/>
       <c r="I123" s="19"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="20"/>
       <c r="B124" s="19"/>
       <c r="C124" s="19"/>
@@ -4109,7 +4120,7 @@
       <c r="H124" s="19"/>
       <c r="I124" s="19"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="20"/>
       <c r="B125" s="19"/>
       <c r="C125" s="19"/>
@@ -4120,7 +4131,7 @@
       <c r="H125" s="19"/>
       <c r="I125" s="19"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="20"/>
       <c r="B126" s="19"/>
       <c r="C126" s="19"/>
@@ -4131,7 +4142,7 @@
       <c r="H126" s="19"/>
       <c r="I126" s="19"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="20"/>
       <c r="B127" s="19"/>
       <c r="C127" s="19"/>
@@ -4142,7 +4153,7 @@
       <c r="H127" s="19"/>
       <c r="I127" s="19"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="20"/>
       <c r="B128" s="19"/>
       <c r="C128" s="19"/>
@@ -4153,7 +4164,7 @@
       <c r="H128" s="19"/>
       <c r="I128" s="19"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="20"/>
       <c r="B129" s="19"/>
       <c r="C129" s="19"/>
@@ -4164,7 +4175,7 @@
       <c r="H129" s="19"/>
       <c r="I129" s="19"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="20"/>
       <c r="B130" s="19"/>
       <c r="C130" s="19"/>
@@ -4175,7 +4186,7 @@
       <c r="H130" s="19"/>
       <c r="I130" s="19"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="20"/>
       <c r="B131" s="19"/>
       <c r="C131" s="19"/>
@@ -4186,7 +4197,7 @@
       <c r="H131" s="19"/>
       <c r="I131" s="19"/>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="20"/>
       <c r="B132" s="19"/>
       <c r="C132" s="19"/>
@@ -4197,7 +4208,7 @@
       <c r="H132" s="19"/>
       <c r="I132" s="19"/>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="20"/>
       <c r="B133" s="19"/>
       <c r="C133" s="19"/>
@@ -4208,7 +4219,7 @@
       <c r="H133" s="19"/>
       <c r="I133" s="19"/>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="20"/>
       <c r="B134" s="19"/>
       <c r="C134" s="19"/>
@@ -4219,7 +4230,7 @@
       <c r="H134" s="19"/>
       <c r="I134" s="19"/>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="20"/>
       <c r="B135" s="19"/>
       <c r="C135" s="19"/>
@@ -4230,7 +4241,7 @@
       <c r="H135" s="19"/>
       <c r="I135" s="19"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="20"/>
       <c r="B136" s="19"/>
       <c r="C136" s="19"/>
@@ -4241,7 +4252,7 @@
       <c r="H136" s="19"/>
       <c r="I136" s="19"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="20"/>
       <c r="B137" s="19"/>
       <c r="C137" s="19"/>
@@ -4252,7 +4263,7 @@
       <c r="H137" s="19"/>
       <c r="I137" s="19"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="20"/>
       <c r="B138" s="19"/>
       <c r="C138" s="19"/>
@@ -4263,7 +4274,7 @@
       <c r="H138" s="19"/>
       <c r="I138" s="19"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="20"/>
       <c r="B139" s="19"/>
       <c r="C139" s="19"/>
@@ -4274,7 +4285,7 @@
       <c r="H139" s="19"/>
       <c r="I139" s="19"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="20"/>
       <c r="B140" s="19"/>
       <c r="C140" s="19"/>
@@ -4285,7 +4296,7 @@
       <c r="H140" s="19"/>
       <c r="I140" s="19"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="20"/>
       <c r="B141" s="19"/>
       <c r="C141" s="19"/>
@@ -4296,7 +4307,7 @@
       <c r="H141" s="19"/>
       <c r="I141" s="19"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="20"/>
       <c r="B142" s="19"/>
       <c r="C142" s="19"/>
@@ -4307,7 +4318,7 @@
       <c r="H142" s="19"/>
       <c r="I142" s="19"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="20"/>
       <c r="B143" s="19"/>
       <c r="C143" s="19"/>
@@ -4318,7 +4329,7 @@
       <c r="H143" s="19"/>
       <c r="I143" s="19"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="20"/>
       <c r="B144" s="19"/>
       <c r="C144" s="19"/>
@@ -4329,7 +4340,7 @@
       <c r="H144" s="19"/>
       <c r="I144" s="19"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="20"/>
       <c r="B145" s="19"/>
       <c r="C145" s="19"/>
@@ -4340,7 +4351,7 @@
       <c r="H145" s="19"/>
       <c r="I145" s="19"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="20"/>
       <c r="B146" s="19"/>
       <c r="C146" s="19"/>
@@ -4351,7 +4362,7 @@
       <c r="H146" s="19"/>
       <c r="I146" s="19"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="20"/>
       <c r="B147" s="19"/>
       <c r="C147" s="19"/>
@@ -4362,7 +4373,7 @@
       <c r="H147" s="19"/>
       <c r="I147" s="19"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="20"/>
       <c r="B148" s="19"/>
       <c r="C148" s="19"/>
@@ -4373,7 +4384,7 @@
       <c r="H148" s="19"/>
       <c r="I148" s="19"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="20"/>
       <c r="B149" s="19"/>
       <c r="C149" s="19"/>
@@ -4384,7 +4395,7 @@
       <c r="H149" s="19"/>
       <c r="I149" s="19"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="20"/>
       <c r="B150" s="19"/>
       <c r="C150" s="19"/>
@@ -4395,7 +4406,7 @@
       <c r="H150" s="19"/>
       <c r="I150" s="19"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="20"/>
       <c r="B151" s="19"/>
       <c r="C151" s="19"/>
@@ -4406,7 +4417,7 @@
       <c r="H151" s="19"/>
       <c r="I151" s="19"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="20"/>
       <c r="B152" s="19"/>
       <c r="C152" s="19"/>
@@ -4417,7 +4428,7 @@
       <c r="H152" s="19"/>
       <c r="I152" s="19"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="20"/>
       <c r="B153" s="19"/>
       <c r="C153" s="19"/>
@@ -4428,7 +4439,7 @@
       <c r="H153" s="19"/>
       <c r="I153" s="19"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="20"/>
       <c r="B154" s="19"/>
       <c r="C154" s="19"/>
@@ -4439,7 +4450,7 @@
       <c r="H154" s="19"/>
       <c r="I154" s="19"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="20"/>
       <c r="B155" s="19"/>
       <c r="C155" s="19"/>
@@ -4450,7 +4461,7 @@
       <c r="H155" s="19"/>
       <c r="I155" s="19"/>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="20"/>
       <c r="B156" s="19"/>
       <c r="C156" s="19"/>
@@ -4461,7 +4472,7 @@
       <c r="H156" s="19"/>
       <c r="I156" s="19"/>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="20"/>
       <c r="B157" s="19"/>
       <c r="C157" s="19"/>
@@ -4472,7 +4483,7 @@
       <c r="H157" s="19"/>
       <c r="I157" s="19"/>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="20"/>
       <c r="B158" s="19"/>
       <c r="C158" s="19"/>
@@ -4483,7 +4494,7 @@
       <c r="H158" s="19"/>
       <c r="I158" s="19"/>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="20"/>
       <c r="B159" s="19"/>
       <c r="C159" s="19"/>
@@ -4494,7 +4505,7 @@
       <c r="H159" s="19"/>
       <c r="I159" s="19"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="20"/>
       <c r="B160" s="19"/>
       <c r="C160" s="19"/>
@@ -4505,7 +4516,7 @@
       <c r="H160" s="19"/>
       <c r="I160" s="19"/>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="20"/>
       <c r="B161" s="19"/>
       <c r="C161" s="19"/>
@@ -4516,7 +4527,7 @@
       <c r="H161" s="19"/>
       <c r="I161" s="19"/>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="20"/>
       <c r="B162" s="19"/>
       <c r="C162" s="19"/>
@@ -4527,7 +4538,7 @@
       <c r="H162" s="19"/>
       <c r="I162" s="19"/>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="20"/>
       <c r="B163" s="19"/>
       <c r="C163" s="19"/>
@@ -4538,7 +4549,7 @@
       <c r="H163" s="19"/>
       <c r="I163" s="19"/>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="20"/>
       <c r="B164" s="19"/>
       <c r="C164" s="19"/>
@@ -4549,7 +4560,7 @@
       <c r="H164" s="19"/>
       <c r="I164" s="19"/>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="20"/>
       <c r="B165" s="19"/>
       <c r="C165" s="19"/>
@@ -4560,7 +4571,7 @@
       <c r="H165" s="19"/>
       <c r="I165" s="19"/>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="20"/>
       <c r="B166" s="19"/>
       <c r="C166" s="19"/>
@@ -4571,7 +4582,7 @@
       <c r="H166" s="19"/>
       <c r="I166" s="19"/>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="20"/>
       <c r="B167" s="19"/>
       <c r="C167" s="19"/>
@@ -4582,7 +4593,7 @@
       <c r="H167" s="19"/>
       <c r="I167" s="19"/>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="20"/>
       <c r="B168" s="19"/>
       <c r="C168" s="19"/>
@@ -4593,7 +4604,7 @@
       <c r="H168" s="19"/>
       <c r="I168" s="19"/>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="20"/>
       <c r="B169" s="19"/>
       <c r="C169" s="19"/>
@@ -4604,7 +4615,7 @@
       <c r="H169" s="19"/>
       <c r="I169" s="19"/>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" s="20"/>
       <c r="B170" s="19"/>
       <c r="C170" s="19"/>
@@ -4615,7 +4626,7 @@
       <c r="H170" s="19"/>
       <c r="I170" s="19"/>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="20"/>
       <c r="B171" s="19"/>
       <c r="C171" s="19"/>
@@ -4626,7 +4637,7 @@
       <c r="H171" s="19"/>
       <c r="I171" s="19"/>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="20"/>
       <c r="B172" s="19"/>
       <c r="C172" s="19"/>
@@ -4637,7 +4648,7 @@
       <c r="H172" s="19"/>
       <c r="I172" s="19"/>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="20"/>
       <c r="B173" s="19"/>
       <c r="C173" s="19"/>
@@ -4648,7 +4659,7 @@
       <c r="H173" s="19"/>
       <c r="I173" s="19"/>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="20"/>
       <c r="B174" s="19"/>
       <c r="C174" s="19"/>
@@ -4659,7 +4670,7 @@
       <c r="H174" s="19"/>
       <c r="I174" s="19"/>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="20"/>
       <c r="B175" s="19"/>
       <c r="C175" s="19"/>
@@ -4670,7 +4681,7 @@
       <c r="H175" s="19"/>
       <c r="I175" s="19"/>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="20"/>
       <c r="B176" s="19"/>
       <c r="C176" s="19"/>
@@ -4681,7 +4692,7 @@
       <c r="H176" s="19"/>
       <c r="I176" s="19"/>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="20"/>
       <c r="B177" s="19"/>
       <c r="C177" s="19"/>
@@ -4692,7 +4703,7 @@
       <c r="H177" s="19"/>
       <c r="I177" s="19"/>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" s="20"/>
       <c r="B178" s="19"/>
       <c r="C178" s="19"/>
@@ -4703,7 +4714,7 @@
       <c r="H178" s="19"/>
       <c r="I178" s="19"/>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="20"/>
       <c r="B179" s="19"/>
       <c r="C179" s="19"/>
@@ -4714,7 +4725,7 @@
       <c r="H179" s="19"/>
       <c r="I179" s="19"/>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="20"/>
       <c r="B180" s="19"/>
       <c r="C180" s="19"/>
@@ -4725,7 +4736,7 @@
       <c r="H180" s="19"/>
       <c r="I180" s="19"/>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" s="20"/>
       <c r="B181" s="19"/>
       <c r="C181" s="19"/>
@@ -4736,7 +4747,7 @@
       <c r="H181" s="19"/>
       <c r="I181" s="19"/>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" s="20"/>
       <c r="B182" s="19"/>
       <c r="C182" s="19"/>
@@ -4747,7 +4758,7 @@
       <c r="H182" s="19"/>
       <c r="I182" s="19"/>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" s="20"/>
       <c r="B183" s="19"/>
       <c r="C183" s="19"/>
@@ -4758,7 +4769,7 @@
       <c r="H183" s="19"/>
       <c r="I183" s="19"/>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" s="20"/>
       <c r="B184" s="19"/>
       <c r="C184" s="19"/>
@@ -4769,7 +4780,7 @@
       <c r="H184" s="19"/>
       <c r="I184" s="19"/>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" s="20"/>
       <c r="B185" s="19"/>
       <c r="C185" s="19"/>
@@ -4780,7 +4791,7 @@
       <c r="H185" s="19"/>
       <c r="I185" s="19"/>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" s="20"/>
       <c r="B186" s="19"/>
       <c r="C186" s="19"/>
@@ -4791,7 +4802,7 @@
       <c r="H186" s="19"/>
       <c r="I186" s="19"/>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" s="20"/>
       <c r="B187" s="19"/>
       <c r="C187" s="19"/>
@@ -4802,7 +4813,7 @@
       <c r="H187" s="19"/>
       <c r="I187" s="19"/>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" s="20"/>
       <c r="B188" s="19"/>
       <c r="C188" s="19"/>
@@ -4813,7 +4824,7 @@
       <c r="H188" s="19"/>
       <c r="I188" s="19"/>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" s="20"/>
       <c r="B189" s="19"/>
       <c r="C189" s="19"/>
@@ -4824,7 +4835,7 @@
       <c r="H189" s="19"/>
       <c r="I189" s="19"/>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" s="20"/>
       <c r="B190" s="19"/>
       <c r="C190" s="19"/>
@@ -4835,7 +4846,7 @@
       <c r="H190" s="19"/>
       <c r="I190" s="19"/>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" s="20"/>
       <c r="B191" s="19"/>
       <c r="C191" s="19"/>
@@ -4846,7 +4857,7 @@
       <c r="H191" s="19"/>
       <c r="I191" s="19"/>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" s="20"/>
       <c r="B192" s="19"/>
       <c r="C192" s="19"/>
@@ -4857,7 +4868,7 @@
       <c r="H192" s="19"/>
       <c r="I192" s="19"/>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" s="20"/>
       <c r="B193" s="19"/>
       <c r="C193" s="19"/>
@@ -4868,7 +4879,7 @@
       <c r="H193" s="19"/>
       <c r="I193" s="19"/>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" s="20"/>
       <c r="B194" s="19"/>
       <c r="C194" s="19"/>
@@ -4879,7 +4890,7 @@
       <c r="H194" s="19"/>
       <c r="I194" s="19"/>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" s="20"/>
       <c r="B195" s="19"/>
       <c r="C195" s="19"/>
@@ -4890,7 +4901,7 @@
       <c r="H195" s="19"/>
       <c r="I195" s="19"/>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" s="20"/>
       <c r="B196" s="19"/>
       <c r="C196" s="19"/>
@@ -4901,7 +4912,7 @@
       <c r="H196" s="19"/>
       <c r="I196" s="19"/>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" s="20"/>
       <c r="B197" s="19"/>
       <c r="C197" s="19"/>
@@ -4912,7 +4923,7 @@
       <c r="H197" s="19"/>
       <c r="I197" s="19"/>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" s="20"/>
       <c r="B198" s="19"/>
       <c r="C198" s="19"/>
@@ -4923,7 +4934,7 @@
       <c r="H198" s="19"/>
       <c r="I198" s="19"/>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" s="20"/>
       <c r="B199" s="19"/>
       <c r="C199" s="19"/>
@@ -4934,7 +4945,7 @@
       <c r="H199" s="19"/>
       <c r="I199" s="19"/>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" s="20"/>
       <c r="B200" s="19"/>
       <c r="C200" s="19"/>
@@ -4945,7 +4956,7 @@
       <c r="H200" s="19"/>
       <c r="I200" s="19"/>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" s="20"/>
       <c r="B201" s="19"/>
       <c r="C201" s="19"/>
@@ -4956,7 +4967,7 @@
       <c r="H201" s="19"/>
       <c r="I201" s="19"/>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" s="20"/>
       <c r="B202" s="19"/>
       <c r="C202" s="19"/>
@@ -4967,7 +4978,7 @@
       <c r="H202" s="19"/>
       <c r="I202" s="19"/>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" s="20"/>
       <c r="B203" s="19"/>
       <c r="C203" s="19"/>
@@ -4978,7 +4989,7 @@
       <c r="H203" s="19"/>
       <c r="I203" s="19"/>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" s="20"/>
       <c r="B204" s="19"/>
       <c r="C204" s="19"/>
@@ -4989,7 +5000,7 @@
       <c r="H204" s="19"/>
       <c r="I204" s="19"/>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" s="20"/>
       <c r="B205" s="19"/>
       <c r="C205" s="19"/>
@@ -5000,7 +5011,7 @@
       <c r="H205" s="19"/>
       <c r="I205" s="19"/>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" s="20"/>
       <c r="B206" s="19"/>
       <c r="C206" s="19"/>
@@ -5011,7 +5022,7 @@
       <c r="H206" s="19"/>
       <c r="I206" s="19"/>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" s="20"/>
       <c r="B207" s="19"/>
       <c r="C207" s="19"/>
@@ -5022,7 +5033,7 @@
       <c r="H207" s="19"/>
       <c r="I207" s="19"/>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" s="20"/>
       <c r="B208" s="19"/>
       <c r="C208" s="19"/>
@@ -5033,7 +5044,7 @@
       <c r="H208" s="19"/>
       <c r="I208" s="19"/>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" s="20"/>
       <c r="B209" s="19"/>
       <c r="C209" s="19"/>
@@ -5044,7 +5055,7 @@
       <c r="H209" s="19"/>
       <c r="I209" s="19"/>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" s="20"/>
       <c r="B210" s="19"/>
       <c r="C210" s="19"/>
@@ -5055,7 +5066,7 @@
       <c r="H210" s="19"/>
       <c r="I210" s="19"/>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" s="20"/>
       <c r="B211" s="19"/>
       <c r="C211" s="19"/>
@@ -5066,7 +5077,7 @@
       <c r="H211" s="19"/>
       <c r="I211" s="19"/>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" s="20"/>
       <c r="B212" s="19"/>
       <c r="C212" s="19"/>
@@ -5077,7 +5088,7 @@
       <c r="H212" s="19"/>
       <c r="I212" s="19"/>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" s="20"/>
       <c r="B213" s="19"/>
       <c r="C213" s="19"/>
@@ -5088,7 +5099,7 @@
       <c r="H213" s="19"/>
       <c r="I213" s="19"/>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" s="20"/>
       <c r="B214" s="19"/>
       <c r="C214" s="19"/>
@@ -5099,7 +5110,7 @@
       <c r="H214" s="19"/>
       <c r="I214" s="19"/>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" s="20"/>
       <c r="B215" s="19"/>
       <c r="C215" s="19"/>
@@ -5110,7 +5121,7 @@
       <c r="H215" s="19"/>
       <c r="I215" s="19"/>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" s="20"/>
       <c r="B216" s="19"/>
       <c r="C216" s="19"/>
@@ -5121,7 +5132,7 @@
       <c r="H216" s="19"/>
       <c r="I216" s="19"/>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" s="20"/>
       <c r="B217" s="19"/>
       <c r="C217" s="19"/>
@@ -5132,7 +5143,7 @@
       <c r="H217" s="19"/>
       <c r="I217" s="19"/>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" s="20"/>
       <c r="B218" s="19"/>
       <c r="C218" s="19"/>
@@ -5143,7 +5154,7 @@
       <c r="H218" s="19"/>
       <c r="I218" s="19"/>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" s="20"/>
       <c r="B219" s="19"/>
       <c r="C219" s="19"/>
@@ -5154,7 +5165,7 @@
       <c r="H219" s="19"/>
       <c r="I219" s="19"/>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" s="20"/>
       <c r="B220" s="19"/>
       <c r="C220" s="19"/>
@@ -5165,7 +5176,7 @@
       <c r="H220" s="19"/>
       <c r="I220" s="19"/>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" s="20"/>
       <c r="B221" s="19"/>
       <c r="C221" s="19"/>
@@ -5176,7 +5187,7 @@
       <c r="H221" s="19"/>
       <c r="I221" s="19"/>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" s="20"/>
       <c r="B222" s="19"/>
       <c r="C222" s="19"/>
@@ -5187,7 +5198,7 @@
       <c r="H222" s="19"/>
       <c r="I222" s="19"/>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" s="20"/>
       <c r="B223" s="19"/>
       <c r="C223" s="19"/>
@@ -5198,7 +5209,7 @@
       <c r="H223" s="19"/>
       <c r="I223" s="19"/>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" s="20"/>
       <c r="B224" s="19"/>
       <c r="C224" s="19"/>
@@ -5209,7 +5220,7 @@
       <c r="H224" s="19"/>
       <c r="I224" s="19"/>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" s="20"/>
       <c r="B225" s="19"/>
       <c r="C225" s="19"/>
@@ -5220,7 +5231,7 @@
       <c r="H225" s="19"/>
       <c r="I225" s="19"/>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" s="20"/>
       <c r="B226" s="19"/>
       <c r="C226" s="19"/>
@@ -5231,7 +5242,7 @@
       <c r="H226" s="19"/>
       <c r="I226" s="19"/>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" s="20"/>
       <c r="B227" s="19"/>
       <c r="C227" s="19"/>
@@ -5242,7 +5253,7 @@
       <c r="H227" s="19"/>
       <c r="I227" s="19"/>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228" s="20"/>
       <c r="B228" s="19"/>
       <c r="C228" s="19"/>
@@ -5253,7 +5264,7 @@
       <c r="H228" s="19"/>
       <c r="I228" s="19"/>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229" s="20"/>
       <c r="B229" s="19"/>
       <c r="C229" s="19"/>
@@ -5264,7 +5275,7 @@
       <c r="H229" s="19"/>
       <c r="I229" s="19"/>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230" s="20"/>
       <c r="B230" s="19"/>
       <c r="C230" s="19"/>
@@ -5275,7 +5286,7 @@
       <c r="H230" s="19"/>
       <c r="I230" s="19"/>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231" s="20"/>
       <c r="B231" s="19"/>
       <c r="C231" s="19"/>
@@ -5286,7 +5297,7 @@
       <c r="H231" s="19"/>
       <c r="I231" s="19"/>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232" s="20"/>
       <c r="B232" s="19"/>
       <c r="C232" s="19"/>
@@ -5297,7 +5308,7 @@
       <c r="H232" s="19"/>
       <c r="I232" s="19"/>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" s="20"/>
       <c r="B233" s="19"/>
       <c r="C233" s="19"/>
@@ -5308,7 +5319,7 @@
       <c r="H233" s="19"/>
       <c r="I233" s="19"/>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234" s="20"/>
       <c r="B234" s="19"/>
       <c r="C234" s="19"/>
@@ -5319,7 +5330,7 @@
       <c r="H234" s="19"/>
       <c r="I234" s="19"/>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" s="20"/>
       <c r="B235" s="19"/>
       <c r="C235" s="19"/>
@@ -5330,7 +5341,7 @@
       <c r="H235" s="19"/>
       <c r="I235" s="19"/>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" s="20"/>
       <c r="B236" s="19"/>
       <c r="C236" s="19"/>
@@ -5341,7 +5352,7 @@
       <c r="H236" s="19"/>
       <c r="I236" s="19"/>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" s="20"/>
       <c r="B237" s="19"/>
       <c r="C237" s="19"/>
@@ -5352,7 +5363,7 @@
       <c r="H237" s="19"/>
       <c r="I237" s="19"/>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A238" s="20"/>
       <c r="B238" s="19"/>
       <c r="C238" s="19"/>
@@ -5363,7 +5374,7 @@
       <c r="H238" s="19"/>
       <c r="I238" s="19"/>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" s="20"/>
       <c r="B239" s="19"/>
       <c r="C239" s="19"/>
@@ -5374,7 +5385,7 @@
       <c r="H239" s="19"/>
       <c r="I239" s="19"/>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240" s="20"/>
       <c r="B240" s="19"/>
       <c r="C240" s="19"/>
@@ -5385,7 +5396,7 @@
       <c r="H240" s="19"/>
       <c r="I240" s="19"/>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241" s="20"/>
       <c r="B241" s="19"/>
       <c r="C241" s="19"/>
@@ -5396,7 +5407,7 @@
       <c r="H241" s="19"/>
       <c r="I241" s="19"/>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242" s="20"/>
       <c r="B242" s="19"/>
       <c r="C242" s="19"/>
@@ -5407,7 +5418,7 @@
       <c r="H242" s="19"/>
       <c r="I242" s="19"/>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243" s="20"/>
       <c r="B243" s="19"/>
       <c r="C243" s="19"/>
@@ -5418,7 +5429,7 @@
       <c r="H243" s="19"/>
       <c r="I243" s="19"/>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244" s="20"/>
       <c r="B244" s="19"/>
       <c r="C244" s="19"/>
@@ -5429,7 +5440,7 @@
       <c r="H244" s="19"/>
       <c r="I244" s="19"/>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245" s="20"/>
       <c r="B245" s="19"/>
       <c r="C245" s="19"/>
@@ -5440,7 +5451,7 @@
       <c r="H245" s="19"/>
       <c r="I245" s="19"/>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246" s="20"/>
       <c r="B246" s="19"/>
       <c r="C246" s="19"/>
@@ -5451,7 +5462,7 @@
       <c r="H246" s="19"/>
       <c r="I246" s="19"/>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247" s="20"/>
       <c r="B247" s="19"/>
       <c r="C247" s="19"/>
@@ -5462,7 +5473,7 @@
       <c r="H247" s="19"/>
       <c r="I247" s="19"/>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248" s="20"/>
       <c r="B248" s="19"/>
       <c r="C248" s="19"/>
@@ -5473,7 +5484,7 @@
       <c r="H248" s="19"/>
       <c r="I248" s="19"/>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249" s="20"/>
       <c r="B249" s="19"/>
       <c r="C249" s="19"/>
@@ -5484,7 +5495,7 @@
       <c r="H249" s="19"/>
       <c r="I249" s="19"/>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" s="20"/>
       <c r="B250" s="19"/>
       <c r="C250" s="19"/>
@@ -5495,7 +5506,7 @@
       <c r="H250" s="19"/>
       <c r="I250" s="19"/>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251" s="20"/>
       <c r="B251" s="19"/>
       <c r="C251" s="19"/>
@@ -5506,7 +5517,7 @@
       <c r="H251" s="19"/>
       <c r="I251" s="19"/>
     </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A252" s="20"/>
       <c r="B252" s="19"/>
       <c r="C252" s="19"/>
@@ -5517,7 +5528,7 @@
       <c r="H252" s="19"/>
       <c r="I252" s="19"/>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253" s="20"/>
       <c r="B253" s="19"/>
       <c r="C253" s="19"/>
@@ -5528,7 +5539,7 @@
       <c r="H253" s="19"/>
       <c r="I253" s="19"/>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254" s="20"/>
       <c r="B254" s="19"/>
       <c r="C254" s="19"/>
@@ -5539,7 +5550,7 @@
       <c r="H254" s="19"/>
       <c r="I254" s="19"/>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255" s="20"/>
       <c r="B255" s="19"/>
       <c r="C255" s="19"/>
@@ -5550,7 +5561,7 @@
       <c r="H255" s="19"/>
       <c r="I255" s="19"/>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256" s="20"/>
       <c r="B256" s="19"/>
       <c r="C256" s="19"/>
@@ -5561,7 +5572,7 @@
       <c r="H256" s="19"/>
       <c r="I256" s="19"/>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A257" s="20"/>
       <c r="B257" s="19"/>
       <c r="C257" s="19"/>
@@ -5572,7 +5583,7 @@
       <c r="H257" s="19"/>
       <c r="I257" s="19"/>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A258" s="20"/>
       <c r="B258" s="19"/>
       <c r="C258" s="19"/>
@@ -5583,7 +5594,7 @@
       <c r="H258" s="19"/>
       <c r="I258" s="19"/>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A259" s="20"/>
       <c r="B259" s="19"/>
       <c r="C259" s="19"/>
@@ -5594,7 +5605,7 @@
       <c r="H259" s="19"/>
       <c r="I259" s="19"/>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A260" s="20"/>
       <c r="B260" s="19"/>
       <c r="C260" s="19"/>
@@ -5605,7 +5616,7 @@
       <c r="H260" s="19"/>
       <c r="I260" s="19"/>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A261" s="20"/>
       <c r="B261" s="19"/>
       <c r="C261" s="19"/>
@@ -5616,7 +5627,7 @@
       <c r="H261" s="19"/>
       <c r="I261" s="19"/>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A262" s="20"/>
       <c r="B262" s="19"/>
       <c r="C262" s="19"/>
@@ -5627,7 +5638,7 @@
       <c r="H262" s="19"/>
       <c r="I262" s="19"/>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A263" s="20"/>
       <c r="B263" s="19"/>
       <c r="C263" s="19"/>
@@ -5638,7 +5649,7 @@
       <c r="H263" s="19"/>
       <c r="I263" s="19"/>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A264" s="20"/>
       <c r="B264" s="19"/>
       <c r="C264" s="19"/>
@@ -5649,7 +5660,7 @@
       <c r="H264" s="19"/>
       <c r="I264" s="19"/>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A265" s="20"/>
       <c r="B265" s="19"/>
       <c r="C265" s="19"/>
@@ -5660,7 +5671,7 @@
       <c r="H265" s="19"/>
       <c r="I265" s="19"/>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A266" s="20"/>
       <c r="B266" s="19"/>
       <c r="C266" s="19"/>
@@ -5671,7 +5682,7 @@
       <c r="H266" s="19"/>
       <c r="I266" s="19"/>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A267" s="20"/>
       <c r="B267" s="19"/>
       <c r="C267" s="19"/>
@@ -5682,7 +5693,7 @@
       <c r="H267" s="19"/>
       <c r="I267" s="19"/>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A268" s="20"/>
       <c r="B268" s="19"/>
       <c r="C268" s="19"/>
@@ -5693,7 +5704,7 @@
       <c r="H268" s="19"/>
       <c r="I268" s="19"/>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A269" s="20"/>
       <c r="B269" s="19"/>
       <c r="C269" s="19"/>
@@ -5704,7 +5715,7 @@
       <c r="H269" s="19"/>
       <c r="I269" s="19"/>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A270" s="20"/>
       <c r="B270" s="19"/>
       <c r="C270" s="19"/>
@@ -5715,7 +5726,7 @@
       <c r="H270" s="19"/>
       <c r="I270" s="19"/>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A271" s="20"/>
       <c r="B271" s="19"/>
       <c r="C271" s="19"/>
@@ -5726,7 +5737,7 @@
       <c r="H271" s="19"/>
       <c r="I271" s="19"/>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A272" s="20"/>
       <c r="B272" s="19"/>
       <c r="C272" s="19"/>
@@ -5737,7 +5748,7 @@
       <c r="H272" s="19"/>
       <c r="I272" s="19"/>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A273" s="20"/>
       <c r="B273" s="19"/>
       <c r="C273" s="19"/>
@@ -5748,7 +5759,7 @@
       <c r="H273" s="19"/>
       <c r="I273" s="19"/>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A274" s="20"/>
       <c r="B274" s="19"/>
       <c r="C274" s="19"/>
@@ -5759,7 +5770,7 @@
       <c r="H274" s="19"/>
       <c r="I274" s="19"/>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A275" s="20"/>
       <c r="B275" s="19"/>
       <c r="C275" s="19"/>
@@ -5770,7 +5781,7 @@
       <c r="H275" s="19"/>
       <c r="I275" s="19"/>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A276" s="20"/>
       <c r="B276" s="19"/>
       <c r="C276" s="19"/>
@@ -5781,7 +5792,7 @@
       <c r="H276" s="19"/>
       <c r="I276" s="19"/>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A277" s="20"/>
       <c r="B277" s="19"/>
       <c r="C277" s="19"/>
@@ -5792,7 +5803,7 @@
       <c r="H277" s="19"/>
       <c r="I277" s="19"/>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A278" s="20"/>
       <c r="B278" s="19"/>
       <c r="C278" s="19"/>
@@ -5803,7 +5814,7 @@
       <c r="H278" s="19"/>
       <c r="I278" s="19"/>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A279" s="20"/>
       <c r="B279" s="19"/>
       <c r="C279" s="19"/>
@@ -5814,7 +5825,7 @@
       <c r="H279" s="19"/>
       <c r="I279" s="19"/>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A280" s="20"/>
       <c r="B280" s="19"/>
       <c r="C280" s="19"/>
@@ -5825,7 +5836,7 @@
       <c r="H280" s="19"/>
       <c r="I280" s="19"/>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A281" s="20"/>
       <c r="B281" s="19"/>
       <c r="C281" s="19"/>
@@ -5836,7 +5847,7 @@
       <c r="H281" s="22"/>
       <c r="I281" s="22"/>
     </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A282" s="20"/>
       <c r="B282" s="19"/>
       <c r="C282" s="19"/>
@@ -5845,7 +5856,7 @@
       <c r="F282" s="23"/>
       <c r="G282" s="23"/>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A283" s="20"/>
       <c r="B283" s="19"/>
       <c r="C283" s="19"/>
@@ -5854,7 +5865,7 @@
       <c r="F283" s="23"/>
       <c r="G283" s="23"/>
     </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A284" s="20"/>
       <c r="B284" s="19"/>
       <c r="C284" s="19"/>
@@ -5863,7 +5874,7 @@
       <c r="F284" s="23"/>
       <c r="G284" s="23"/>
     </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A285" s="20"/>
       <c r="B285" s="19"/>
       <c r="C285" s="19"/>
@@ -5872,7 +5883,7 @@
       <c r="F285" s="23"/>
       <c r="G285" s="23"/>
     </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A286" s="20"/>
       <c r="B286" s="19"/>
       <c r="C286" s="19"/>
@@ -5881,7 +5892,7 @@
       <c r="F286" s="23"/>
       <c r="G286" s="23"/>
     </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A287" s="20"/>
       <c r="B287" s="19"/>
       <c r="C287" s="19"/>
@@ -5890,7 +5901,7 @@
       <c r="F287" s="23"/>
       <c r="G287" s="23"/>
     </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A288" s="20"/>
       <c r="B288" s="19"/>
       <c r="C288" s="19"/>
@@ -5899,7 +5910,7 @@
       <c r="F288" s="23"/>
       <c r="G288" s="23"/>
     </row>
-    <row r="289" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A289" s="20"/>
       <c r="B289" s="19"/>
       <c r="C289" s="19"/>
@@ -5908,7 +5919,7 @@
       <c r="F289" s="23"/>
       <c r="G289" s="23"/>
     </row>
-    <row r="290" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A290" s="20"/>
       <c r="B290" s="19"/>
       <c r="C290" s="19"/>
@@ -5917,7 +5928,7 @@
       <c r="F290" s="23"/>
       <c r="G290" s="23"/>
     </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A291" s="20"/>
       <c r="B291" s="19"/>
       <c r="C291" s="19"/>
@@ -5926,7 +5937,7 @@
       <c r="F291" s="23"/>
       <c r="G291" s="23"/>
     </row>
-    <row r="292" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A292" s="20"/>
       <c r="B292" s="19"/>
       <c r="C292" s="19"/>
@@ -5935,7 +5946,7 @@
       <c r="F292" s="23"/>
       <c r="G292" s="23"/>
     </row>
-    <row r="293" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A293" s="20"/>
       <c r="B293" s="19"/>
       <c r="C293" s="19"/>
@@ -5944,7 +5955,7 @@
       <c r="F293" s="23"/>
       <c r="G293" s="23"/>
     </row>
-    <row r="294" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A294" s="20"/>
       <c r="B294" s="19"/>
       <c r="C294" s="19"/>
@@ -5953,7 +5964,7 @@
       <c r="F294" s="23"/>
       <c r="G294" s="23"/>
     </row>
-    <row r="295" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A295" s="20"/>
       <c r="B295" s="19"/>
       <c r="C295" s="19"/>
@@ -5962,7 +5973,7 @@
       <c r="F295" s="23"/>
       <c r="G295" s="23"/>
     </row>
-    <row r="296" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A296" s="20"/>
       <c r="B296" s="19"/>
       <c r="C296" s="19"/>
@@ -5971,7 +5982,7 @@
       <c r="F296" s="23"/>
       <c r="G296" s="23"/>
     </row>
-    <row r="297" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A297" s="20"/>
       <c r="B297" s="19"/>
       <c r="C297" s="19"/>
@@ -5980,7 +5991,7 @@
       <c r="F297" s="23"/>
       <c r="G297" s="23"/>
     </row>
-    <row r="298" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A298" s="20"/>
       <c r="B298" s="19"/>
       <c r="C298" s="19"/>
@@ -5989,7 +6000,7 @@
       <c r="F298" s="23"/>
       <c r="G298" s="23"/>
     </row>
-    <row r="299" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A299" s="20"/>
       <c r="B299" s="19"/>
       <c r="C299" s="19"/>
@@ -5998,7 +6009,7 @@
       <c r="F299" s="23"/>
       <c r="G299" s="23"/>
     </row>
-    <row r="300" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A300" s="20"/>
       <c r="B300" s="19"/>
       <c r="C300" s="19"/>
@@ -6007,7 +6018,7 @@
       <c r="F300" s="23"/>
       <c r="G300" s="23"/>
     </row>
-    <row r="301" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A301" s="20"/>
       <c r="B301" s="19"/>
       <c r="C301" s="19"/>
@@ -6016,7 +6027,7 @@
       <c r="F301" s="23"/>
       <c r="G301" s="23"/>
     </row>
-    <row r="302" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A302" s="20"/>
       <c r="B302" s="19"/>
       <c r="C302" s="19"/>
@@ -6025,7 +6036,7 @@
       <c r="F302" s="23"/>
       <c r="G302" s="23"/>
     </row>
-    <row r="303" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A303" s="20"/>
       <c r="B303" s="19"/>
       <c r="C303" s="19"/>
@@ -6034,7 +6045,7 @@
       <c r="F303" s="23"/>
       <c r="G303" s="23"/>
     </row>
-    <row r="304" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A304" s="20"/>
       <c r="B304" s="19"/>
       <c r="C304" s="22"/>
@@ -6043,7 +6054,7 @@
       <c r="F304" s="23"/>
       <c r="G304" s="23"/>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A305" s="21"/>
       <c r="B305" s="22"/>
     </row>
@@ -6059,11 +6070,11 @@
     <mergeCell ref="F2:G2"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A64 A71:A515" xr:uid="{140C1EC3-30A5-2448-BEAA-24AD135906D1}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A64 A71:A515">
       <formula1>43831</formula1>
       <formula2>44561</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I299 H63:H299 H5:H60 B5:B64 B71:B323 C5:C322" xr:uid="{41FC32AD-2E84-E042-9905-63CAE446C667}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I299 H63:H299 H5:H60 B5:B64 B71:B323 C5:C322">
       <formula1>0</formula1>
       <formula2>10000000</formula2>
     </dataValidation>
@@ -6073,41 +6084,41 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE078372-B08E-3945-8236-75FE2E0407AC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.375" customWidth="1"/>
+    <col min="4" max="4" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C4" s="45" t="s">
         <v>79</v>
       </c>
       <c r="D4" s="46"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>12</v>
       </c>
@@ -6121,7 +6132,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>75</v>
       </c>
@@ -6135,7 +6146,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>76</v>
       </c>
@@ -6149,7 +6160,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>77</v>
       </c>
@@ -6163,7 +6174,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>78</v>
       </c>
@@ -6177,16 +6188,16 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C4:D4"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:D9" xr:uid="{16C39E30-A382-9841-B9C1-7BE92A80BACE}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:D9">
       <formula1>0</formula1>
       <formula2>20</formula2>
     </dataValidation>
@@ -6196,21 +6207,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99DD5F9C-4676-5749-AB11-9739EC646DB2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1640625" customWidth="1"/>
+    <col min="1" max="1" width="25.125" customWidth="1"/>
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -6224,7 +6235,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>15</v>
       </c>
@@ -6235,7 +6246,7 @@
         <v>12345</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>16</v>
       </c>
@@ -6249,7 +6260,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>18</v>
       </c>
@@ -6263,7 +6274,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>17</v>
       </c>
@@ -6274,7 +6285,7 @@
         <v>43877</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>23</v>
       </c>
@@ -6288,7 +6299,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>24</v>
       </c>
@@ -6302,7 +6313,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>37</v>
       </c>
@@ -6316,7 +6327,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>38</v>
       </c>
@@ -6328,7 +6339,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>39</v>
       </c>
@@ -6339,7 +6350,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>40</v>
       </c>
@@ -6353,7 +6364,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
         <v>41</v>
       </c>
@@ -6367,7 +6378,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>82</v>
       </c>
@@ -6380,15 +6391,15 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{8AA04D2D-EF0D-8145-8E7C-689CB89575F4}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>1</formula1>
       <formula2>10000000</formula2>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{68A0B7A5-3DC8-EB48-B02F-9DB169C81F40}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
       <formula1>43831</formula1>
       <formula2>44561</formula2>
     </dataValidation>
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="B4 B6:B7" xr:uid="{45601BFC-E9DB-8A44-9B12-B2E34605D44B}">
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="B4 B6:B7">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
update San Francisco and Santa Cruz
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10614"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris_hoover\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{36CE5D05-39BB-3143-B6F5-79528135F815}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4155" yWindow="720" windowWidth="29445" windowHeight="19500" activeTab="3"/>
+    <workbookView xWindow="4160" yWindow="720" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters with Distributions" sheetId="1" r:id="rId1"/>
@@ -280,13 +281,13 @@
     <t>lambda_ini_exposed</t>
   </si>
   <si>
-    <t>~/Documents/GitHub/LEMMA-Forecasts/Forecasts/San Francisco</t>
+    <t>Forecasts/San Francisco</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -883,22 +884,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" style="30" customWidth="1"/>
     <col min="2" max="2" width="62.5" style="2" customWidth="1"/>
-    <col min="3" max="4" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.875" style="1"/>
+    <col min="3" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
         <v>12</v>
       </c>
@@ -912,7 +913,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
         <v>73</v>
       </c>
@@ -926,7 +927,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
         <v>74</v>
       </c>
@@ -940,7 +941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
         <v>45</v>
       </c>
@@ -954,7 +955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="30" t="s">
         <v>46</v>
       </c>
@@ -968,7 +969,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="30" t="s">
         <v>47</v>
       </c>
@@ -982,7 +983,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="30" t="s">
         <v>48</v>
       </c>
@@ -996,7 +997,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="30" t="s">
         <v>44</v>
       </c>
@@ -1010,7 +1011,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="s">
         <v>51</v>
       </c>
@@ -1024,7 +1025,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="30" t="s">
         <v>52</v>
       </c>
@@ -1040,11 +1041,11 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D2">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D2" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
       <formula2>20</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:D10">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:D10" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -1054,21 +1055,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="10.375" customWidth="1"/>
-    <col min="4" max="4" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.375" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
         <v>57</v>
       </c>
@@ -1082,7 +1083,7 @@
       </c>
       <c r="F1" s="38"/>
     </row>
-    <row r="2" spans="1:6" s="28" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="28" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
         <v>35</v>
       </c>
@@ -1102,7 +1103,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
         <v>67</v>
       </c>
@@ -1122,7 +1123,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>43897</v>
       </c>
@@ -1142,7 +1143,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>43907</v>
       </c>
@@ -1162,7 +1163,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>43927</v>
       </c>
@@ -1182,7 +1183,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>43941</v>
       </c>
@@ -1202,7 +1203,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>43955</v>
       </c>
@@ -1222,7 +1223,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>43969</v>
       </c>
@@ -1242,7 +1243,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>43983</v>
       </c>
@@ -1262,7 +1263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>43997</v>
       </c>
@@ -1289,11 +1290,11 @@
     <mergeCell ref="E1:F1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A11">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A11" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>43831</formula1>
       <formula2>44196</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>0</formula1>
       <formula2>30</formula2>
     </dataValidation>
@@ -1303,20 +1304,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
@@ -1327,7 +1328,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -1338,7 +1339,7 @@
         <v>883305</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>21</v>
       </c>
@@ -1349,7 +1350,7 @@
         <v>43905</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
@@ -1362,11 +1363,11 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="C2">
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>0</formula1>
       <formula2>100000000</formula2>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C4">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C4" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>43831</formula1>
       <formula2>44561</formula2>
     </dataValidation>
@@ -1376,28 +1377,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I305"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="20" topLeftCell="G112" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="20" topLeftCell="G105" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="F114" sqref="F114"/>
+      <selection pane="bottomRight" activeCell="E116" sqref="E116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="45.5" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.125" style="3" customWidth="1"/>
-    <col min="4" max="7" width="12.875" customWidth="1"/>
-    <col min="8" max="8" width="12.875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" style="3" customWidth="1"/>
+    <col min="4" max="7" width="12.83203125" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" style="3" customWidth="1"/>
     <col min="9" max="9" width="14.5" style="3" customWidth="1"/>
     <col min="10" max="10" width="45.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="16"/>
       <c r="B1" s="42" t="s">
         <v>25</v>
@@ -1416,7 +1417,7 @@
       </c>
       <c r="I1" s="39"/>
     </row>
-    <row r="2" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="41" t="s">
         <v>29</v>
       </c>
@@ -1434,7 +1435,7 @@
       </c>
       <c r="I2" s="40"/>
     </row>
-    <row r="3" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>5</v>
       </c>
@@ -1463,7 +1464,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
         <v>28</v>
       </c>
@@ -1492,7 +1493,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="18">
         <v>43913</v>
       </c>
@@ -1515,7 +1516,7 @@
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="18">
         <v>43914</v>
       </c>
@@ -1538,7 +1539,7 @@
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="18">
         <v>43915</v>
       </c>
@@ -1561,7 +1562,7 @@
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="18">
         <v>43916</v>
       </c>
@@ -1584,7 +1585,7 @@
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="18">
         <v>43917</v>
       </c>
@@ -1607,7 +1608,7 @@
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="18">
         <v>43918</v>
       </c>
@@ -1630,7 +1631,7 @@
       <c r="H10" s="19"/>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="18">
         <v>43919</v>
       </c>
@@ -1653,7 +1654,7 @@
       <c r="H11" s="23"/>
       <c r="I11" s="19"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="18">
         <v>43920</v>
       </c>
@@ -1676,7 +1677,7 @@
       <c r="H12" s="23"/>
       <c r="I12" s="19"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
         <v>43921</v>
       </c>
@@ -1699,7 +1700,7 @@
       <c r="H13" s="23"/>
       <c r="I13" s="19"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="18">
         <v>43922</v>
       </c>
@@ -1722,7 +1723,7 @@
       <c r="H14" s="23"/>
       <c r="I14" s="19"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="18">
         <v>43923</v>
       </c>
@@ -1745,7 +1746,7 @@
       <c r="H15" s="23"/>
       <c r="I15" s="19"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
         <v>43924</v>
       </c>
@@ -1768,7 +1769,7 @@
       <c r="H16" s="23"/>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="18">
         <v>43925</v>
       </c>
@@ -1791,7 +1792,7 @@
       <c r="H17" s="23"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="18">
         <v>43926</v>
       </c>
@@ -1814,7 +1815,7 @@
       <c r="H18" s="23"/>
       <c r="I18" s="19"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="18">
         <v>43927</v>
       </c>
@@ -1837,7 +1838,7 @@
       <c r="H19" s="23"/>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="20">
         <v>43928</v>
       </c>
@@ -1860,7 +1861,7 @@
       <c r="H20" s="23"/>
       <c r="I20" s="19"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="20">
         <v>43929</v>
       </c>
@@ -1883,7 +1884,7 @@
       <c r="H21" s="23"/>
       <c r="I21" s="19"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="20">
         <v>43930</v>
       </c>
@@ -1906,7 +1907,7 @@
       <c r="H22" s="23"/>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="20">
         <v>43931</v>
       </c>
@@ -1929,7 +1930,7 @@
       <c r="H23" s="23"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="20">
         <v>43932</v>
       </c>
@@ -1952,7 +1953,7 @@
       <c r="H24" s="23"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="20">
         <v>43933</v>
       </c>
@@ -1975,7 +1976,7 @@
       <c r="H25" s="23"/>
       <c r="I25" s="19"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="20">
         <v>43934</v>
       </c>
@@ -1998,7 +1999,7 @@
       <c r="H26" s="23"/>
       <c r="I26" s="19"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="20">
         <v>43935</v>
       </c>
@@ -2021,7 +2022,7 @@
       <c r="H27" s="23"/>
       <c r="I27" s="19"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="20">
         <v>43936</v>
       </c>
@@ -2044,7 +2045,7 @@
       <c r="H28" s="23"/>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="20">
         <v>43937</v>
       </c>
@@ -2067,7 +2068,7 @@
       <c r="H29" s="23"/>
       <c r="I29" s="19"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="20">
         <v>43938</v>
       </c>
@@ -2090,7 +2091,7 @@
       <c r="H30" s="23"/>
       <c r="I30" s="19"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="20">
         <v>43939</v>
       </c>
@@ -2113,7 +2114,7 @@
       <c r="H31" s="23"/>
       <c r="I31" s="19"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="20">
         <v>43940</v>
       </c>
@@ -2136,7 +2137,7 @@
       <c r="H32" s="23"/>
       <c r="I32" s="19"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="20">
         <v>43941</v>
       </c>
@@ -2159,7 +2160,7 @@
       <c r="H33" s="23"/>
       <c r="I33" s="19"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="20">
         <v>43942</v>
       </c>
@@ -2182,7 +2183,7 @@
       <c r="H34" s="23"/>
       <c r="I34" s="19"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="20">
         <v>43943</v>
       </c>
@@ -2205,7 +2206,7 @@
       <c r="H35" s="23"/>
       <c r="I35" s="19"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="20">
         <v>43944</v>
       </c>
@@ -2228,7 +2229,7 @@
       <c r="H36" s="23"/>
       <c r="I36" s="19"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="20">
         <v>43945</v>
       </c>
@@ -2251,7 +2252,7 @@
       <c r="H37" s="23"/>
       <c r="I37" s="19"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="20">
         <v>43946</v>
       </c>
@@ -2274,7 +2275,7 @@
       <c r="H38" s="23"/>
       <c r="I38" s="19"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="20">
         <v>43947</v>
       </c>
@@ -2297,7 +2298,7 @@
       <c r="H39" s="23"/>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="20">
         <v>43948</v>
       </c>
@@ -2320,7 +2321,7 @@
       <c r="H40" s="23"/>
       <c r="I40" s="19"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="20">
         <v>43949</v>
       </c>
@@ -2343,7 +2344,7 @@
       <c r="H41" s="23"/>
       <c r="I41" s="19"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="20">
         <v>43950</v>
       </c>
@@ -2366,7 +2367,7 @@
       <c r="H42" s="23"/>
       <c r="I42" s="19"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="20">
         <v>43951</v>
       </c>
@@ -2389,7 +2390,7 @@
       <c r="H43" s="23"/>
       <c r="I43" s="19"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="20">
         <v>43952</v>
       </c>
@@ -2412,7 +2413,7 @@
       <c r="H44" s="23"/>
       <c r="I44" s="19"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="20">
         <v>43953</v>
       </c>
@@ -2435,7 +2436,7 @@
       <c r="H45" s="23"/>
       <c r="I45" s="19"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="20">
         <v>43954</v>
       </c>
@@ -2458,7 +2459,7 @@
       <c r="H46" s="23"/>
       <c r="I46" s="19"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="20">
         <v>43955</v>
       </c>
@@ -2481,7 +2482,7 @@
       <c r="H47" s="23"/>
       <c r="I47" s="19"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="20">
         <v>43956</v>
       </c>
@@ -2504,7 +2505,7 @@
       <c r="H48" s="23"/>
       <c r="I48" s="19"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="20">
         <v>43957</v>
       </c>
@@ -2527,7 +2528,7 @@
       <c r="H49" s="23"/>
       <c r="I49" s="19"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="20">
         <v>43958</v>
       </c>
@@ -2550,7 +2551,7 @@
       <c r="H50" s="23"/>
       <c r="I50" s="19"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="20">
         <v>43959</v>
       </c>
@@ -2573,7 +2574,7 @@
       <c r="H51" s="23"/>
       <c r="I51" s="19"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="20">
         <v>43960</v>
       </c>
@@ -2596,7 +2597,7 @@
       <c r="H52" s="23"/>
       <c r="I52" s="19"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="20">
         <v>43961</v>
       </c>
@@ -2619,7 +2620,7 @@
       <c r="H53" s="23"/>
       <c r="I53" s="19"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="20">
         <v>43962</v>
       </c>
@@ -2642,7 +2643,7 @@
       <c r="H54" s="23"/>
       <c r="I54" s="19"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="20">
         <v>43963</v>
       </c>
@@ -2665,7 +2666,7 @@
       <c r="H55" s="23"/>
       <c r="I55" s="19"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="20">
         <v>43964</v>
       </c>
@@ -2688,7 +2689,7 @@
       <c r="H56" s="23"/>
       <c r="I56" s="19"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="20">
         <v>43965</v>
       </c>
@@ -2711,7 +2712,7 @@
       <c r="H57" s="23"/>
       <c r="I57" s="19"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="20">
         <v>43966</v>
       </c>
@@ -2734,7 +2735,7 @@
       <c r="H58" s="23"/>
       <c r="I58" s="19"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="20">
         <v>43967</v>
       </c>
@@ -2757,7 +2758,7 @@
       <c r="H59" s="23"/>
       <c r="I59" s="19"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="20">
         <v>43968</v>
       </c>
@@ -2780,7 +2781,7 @@
       <c r="H60" s="23"/>
       <c r="I60" s="19"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="20">
         <v>43969</v>
       </c>
@@ -2803,7 +2804,7 @@
       <c r="H61" s="23"/>
       <c r="I61" s="19"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="20">
         <v>43970</v>
       </c>
@@ -2826,7 +2827,7 @@
       <c r="H62" s="23"/>
       <c r="I62" s="19"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="20">
         <v>43971</v>
       </c>
@@ -2849,7 +2850,7 @@
       <c r="H63" s="23"/>
       <c r="I63" s="19"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="20">
         <v>43972</v>
       </c>
@@ -2872,7 +2873,7 @@
       <c r="H64" s="23"/>
       <c r="I64" s="19"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="24">
         <v>43973</v>
       </c>
@@ -2895,7 +2896,7 @@
       <c r="H65" s="23"/>
       <c r="I65" s="19"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="24">
         <v>43974</v>
       </c>
@@ -2918,7 +2919,7 @@
       <c r="H66" s="19"/>
       <c r="I66" s="19"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="24">
         <v>43975</v>
       </c>
@@ -2941,7 +2942,7 @@
       <c r="H67" s="19"/>
       <c r="I67" s="19"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="24">
         <v>43976</v>
       </c>
@@ -2964,7 +2965,7 @@
       <c r="H68" s="19"/>
       <c r="I68" s="19"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="24">
         <v>43977</v>
       </c>
@@ -2987,7 +2988,7 @@
       <c r="H69" s="19"/>
       <c r="I69" s="19"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="24">
         <v>43978</v>
       </c>
@@ -3010,7 +3011,7 @@
       <c r="H70" s="19"/>
       <c r="I70" s="19"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="20">
         <v>43979</v>
       </c>
@@ -3033,7 +3034,7 @@
       <c r="H71" s="19"/>
       <c r="I71" s="19"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="20">
         <v>43980</v>
       </c>
@@ -3056,7 +3057,7 @@
       <c r="H72" s="19"/>
       <c r="I72" s="19"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="20">
         <v>43981</v>
       </c>
@@ -3079,7 +3080,7 @@
       <c r="H73" s="19"/>
       <c r="I73" s="19"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="20">
         <v>43982</v>
       </c>
@@ -3102,7 +3103,7 @@
       <c r="H74" s="19"/>
       <c r="I74" s="19"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="20">
         <v>43983</v>
       </c>
@@ -3125,7 +3126,7 @@
       <c r="H75" s="19"/>
       <c r="I75" s="19"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="20">
         <v>43984</v>
       </c>
@@ -3148,7 +3149,7 @@
       <c r="H76" s="19"/>
       <c r="I76" s="19"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="20">
         <v>43985</v>
       </c>
@@ -3171,7 +3172,7 @@
       <c r="H77" s="19"/>
       <c r="I77" s="19"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="20">
         <v>43986</v>
       </c>
@@ -3194,7 +3195,7 @@
       <c r="H78" s="19"/>
       <c r="I78" s="19"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="20">
         <v>43987</v>
       </c>
@@ -3217,7 +3218,7 @@
       <c r="H79" s="19"/>
       <c r="I79" s="19"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="20">
         <v>43988</v>
       </c>
@@ -3240,7 +3241,7 @@
       <c r="H80" s="19"/>
       <c r="I80" s="19"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="20">
         <v>43989</v>
       </c>
@@ -3263,7 +3264,7 @@
       <c r="H81" s="19"/>
       <c r="I81" s="19"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="20">
         <v>43990</v>
       </c>
@@ -3286,7 +3287,7 @@
       <c r="H82" s="19"/>
       <c r="I82" s="19"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="20">
         <v>43991</v>
       </c>
@@ -3309,7 +3310,7 @@
       <c r="H83" s="19"/>
       <c r="I83" s="19"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="20">
         <v>43992</v>
       </c>
@@ -3332,7 +3333,7 @@
       <c r="H84" s="19"/>
       <c r="I84" s="19"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="20">
         <v>43993</v>
       </c>
@@ -3355,7 +3356,7 @@
       <c r="H85" s="19"/>
       <c r="I85" s="19"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="20">
         <v>43994</v>
       </c>
@@ -3378,7 +3379,7 @@
       <c r="H86" s="19"/>
       <c r="I86" s="19"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="20">
         <v>43995</v>
       </c>
@@ -3401,7 +3402,7 @@
       <c r="H87" s="19"/>
       <c r="I87" s="19"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="20">
         <v>43996</v>
       </c>
@@ -3424,7 +3425,7 @@
       <c r="H88" s="19"/>
       <c r="I88" s="19"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="20">
         <v>43997</v>
       </c>
@@ -3447,7 +3448,7 @@
       <c r="H89" s="19"/>
       <c r="I89" s="19"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="20">
         <v>43998</v>
       </c>
@@ -3470,7 +3471,7 @@
       <c r="H90" s="19"/>
       <c r="I90" s="19"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="20">
         <v>43999</v>
       </c>
@@ -3493,7 +3494,7 @@
       <c r="H91" s="19"/>
       <c r="I91" s="19"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="20">
         <v>44000</v>
       </c>
@@ -3516,7 +3517,7 @@
       <c r="H92" s="19"/>
       <c r="I92" s="19"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="20">
         <v>44001</v>
       </c>
@@ -3539,7 +3540,7 @@
       <c r="H93" s="19"/>
       <c r="I93" s="19"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="20">
         <v>44002</v>
       </c>
@@ -3562,7 +3563,7 @@
       <c r="H94" s="19"/>
       <c r="I94" s="19"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="20">
         <v>44003</v>
       </c>
@@ -3585,7 +3586,7 @@
       <c r="H95" s="19"/>
       <c r="I95" s="19"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="20">
         <v>44004</v>
       </c>
@@ -3608,7 +3609,7 @@
       <c r="H96" s="19"/>
       <c r="I96" s="19"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" s="20">
         <v>44005</v>
       </c>
@@ -3631,7 +3632,7 @@
       <c r="H97" s="19"/>
       <c r="I97" s="19"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="20">
         <v>44006</v>
       </c>
@@ -3654,7 +3655,7 @@
       <c r="H98" s="19"/>
       <c r="I98" s="19"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="20">
         <v>44007</v>
       </c>
@@ -3677,7 +3678,7 @@
       <c r="H99" s="19"/>
       <c r="I99" s="19"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" s="20">
         <v>44008</v>
       </c>
@@ -3700,7 +3701,7 @@
       <c r="H100" s="19"/>
       <c r="I100" s="19"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" s="20">
         <v>44009</v>
       </c>
@@ -3723,7 +3724,7 @@
       <c r="H101" s="19"/>
       <c r="I101" s="19"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" s="20">
         <v>44010</v>
       </c>
@@ -3746,7 +3747,7 @@
       <c r="H102" s="19"/>
       <c r="I102" s="19"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" s="20">
         <v>44011</v>
       </c>
@@ -3769,7 +3770,7 @@
       <c r="H103" s="19"/>
       <c r="I103" s="19"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" s="20">
         <v>44012</v>
       </c>
@@ -3792,7 +3793,7 @@
       <c r="H104" s="19"/>
       <c r="I104" s="19"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" s="20">
         <v>44013</v>
       </c>
@@ -3815,7 +3816,7 @@
       <c r="H105" s="19"/>
       <c r="I105" s="19"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" s="20">
         <v>44014</v>
       </c>
@@ -3838,7 +3839,7 @@
       <c r="H106" s="19"/>
       <c r="I106" s="19"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" s="20">
         <v>44015</v>
       </c>
@@ -3861,7 +3862,7 @@
       <c r="H107" s="19"/>
       <c r="I107" s="19"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" s="20">
         <v>44016</v>
       </c>
@@ -3869,10 +3870,10 @@
         <v>53</v>
       </c>
       <c r="C108" s="19">
+        <v>11</v>
+      </c>
+      <c r="D108" s="23">
         <v>15</v>
-      </c>
-      <c r="D108" s="23">
-        <v>11</v>
       </c>
       <c r="E108" s="23">
         <v>1</v>
@@ -3884,7 +3885,7 @@
       <c r="H108" s="19"/>
       <c r="I108" s="19"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" s="20">
         <v>44017</v>
       </c>
@@ -3892,10 +3893,10 @@
         <v>55</v>
       </c>
       <c r="C109" s="19">
+        <v>13</v>
+      </c>
+      <c r="D109" s="23">
         <v>17</v>
-      </c>
-      <c r="D109" s="23">
-        <v>13</v>
       </c>
       <c r="E109" s="23">
         <v>1</v>
@@ -3907,7 +3908,7 @@
       <c r="H109" s="19"/>
       <c r="I109" s="19"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" s="20">
         <v>44018</v>
       </c>
@@ -3930,7 +3931,7 @@
       <c r="H110" s="19"/>
       <c r="I110" s="19"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" s="20">
         <v>44019</v>
       </c>
@@ -3953,18 +3954,18 @@
       <c r="H111" s="19"/>
       <c r="I111" s="19"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" s="20">
         <v>44020</v>
       </c>
       <c r="B112" s="19">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C112" s="19">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D112" s="23">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E112" s="23">
         <v>2</v>
@@ -3976,7 +3977,7 @@
       <c r="H112" s="19"/>
       <c r="I112" s="19"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" s="20">
         <v>44021</v>
       </c>
@@ -3984,7 +3985,7 @@
         <v>59</v>
       </c>
       <c r="C113" s="19">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D113" s="23">
         <v>19</v>
@@ -3999,29 +4000,53 @@
       <c r="H113" s="19"/>
       <c r="I113" s="19"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A114" s="20"/>
-      <c r="B114" s="19"/>
-      <c r="C114" s="19"/>
-      <c r="D114" s="23"/>
-      <c r="E114" s="23"/>
-      <c r="F114" s="23"/>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A114" s="20">
+        <v>44022</v>
+      </c>
+      <c r="B114" s="19">
+        <v>62</v>
+      </c>
+      <c r="C114" s="19">
+        <v>21</v>
+      </c>
+      <c r="D114" s="23">
+        <v>22</v>
+      </c>
+      <c r="E114" s="23">
+        <v>2</v>
+      </c>
+      <c r="F114" s="23">
+        <v>50</v>
+      </c>
       <c r="G114" s="23"/>
       <c r="H114" s="19"/>
       <c r="I114" s="19"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A115" s="20"/>
-      <c r="B115" s="19"/>
-      <c r="C115" s="19"/>
-      <c r="D115" s="23"/>
-      <c r="E115" s="23"/>
-      <c r="F115" s="23"/>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A115" s="20">
+        <v>44023</v>
+      </c>
+      <c r="B115" s="19">
+        <v>68</v>
+      </c>
+      <c r="C115" s="19">
+        <v>13</v>
+      </c>
+      <c r="D115" s="23">
+        <v>24</v>
+      </c>
+      <c r="E115" s="23">
+        <v>1</v>
+      </c>
+      <c r="F115" s="23">
+        <v>50</v>
+      </c>
       <c r="G115" s="23"/>
       <c r="H115" s="19"/>
       <c r="I115" s="19"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" s="20"/>
       <c r="B116" s="19"/>
       <c r="C116" s="19"/>
@@ -4032,7 +4057,7 @@
       <c r="H116" s="19"/>
       <c r="I116" s="19"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" s="20"/>
       <c r="B117" s="19"/>
       <c r="C117" s="19"/>
@@ -4043,7 +4068,7 @@
       <c r="H117" s="19"/>
       <c r="I117" s="19"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" s="20"/>
       <c r="B118" s="19"/>
       <c r="C118" s="19"/>
@@ -4054,7 +4079,7 @@
       <c r="H118" s="19"/>
       <c r="I118" s="19"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" s="20"/>
       <c r="B119" s="19"/>
       <c r="C119" s="19"/>
@@ -4065,7 +4090,7 @@
       <c r="H119" s="19"/>
       <c r="I119" s="19"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" s="20"/>
       <c r="B120" s="19"/>
       <c r="C120" s="19"/>
@@ -4076,7 +4101,7 @@
       <c r="H120" s="19"/>
       <c r="I120" s="19"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" s="20"/>
       <c r="B121" s="19"/>
       <c r="C121" s="19"/>
@@ -4087,7 +4112,7 @@
       <c r="H121" s="19"/>
       <c r="I121" s="19"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" s="20"/>
       <c r="B122" s="19"/>
       <c r="C122" s="19"/>
@@ -4098,7 +4123,7 @@
       <c r="H122" s="19"/>
       <c r="I122" s="19"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" s="20"/>
       <c r="B123" s="19"/>
       <c r="C123" s="19"/>
@@ -4109,7 +4134,7 @@
       <c r="H123" s="19"/>
       <c r="I123" s="19"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" s="20"/>
       <c r="B124" s="19"/>
       <c r="C124" s="19"/>
@@ -4120,7 +4145,7 @@
       <c r="H124" s="19"/>
       <c r="I124" s="19"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" s="20"/>
       <c r="B125" s="19"/>
       <c r="C125" s="19"/>
@@ -4131,7 +4156,7 @@
       <c r="H125" s="19"/>
       <c r="I125" s="19"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" s="20"/>
       <c r="B126" s="19"/>
       <c r="C126" s="19"/>
@@ -4142,7 +4167,7 @@
       <c r="H126" s="19"/>
       <c r="I126" s="19"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" s="20"/>
       <c r="B127" s="19"/>
       <c r="C127" s="19"/>
@@ -4153,7 +4178,7 @@
       <c r="H127" s="19"/>
       <c r="I127" s="19"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" s="20"/>
       <c r="B128" s="19"/>
       <c r="C128" s="19"/>
@@ -4164,7 +4189,7 @@
       <c r="H128" s="19"/>
       <c r="I128" s="19"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129" s="20"/>
       <c r="B129" s="19"/>
       <c r="C129" s="19"/>
@@ -4175,7 +4200,7 @@
       <c r="H129" s="19"/>
       <c r="I129" s="19"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" s="20"/>
       <c r="B130" s="19"/>
       <c r="C130" s="19"/>
@@ -4186,7 +4211,7 @@
       <c r="H130" s="19"/>
       <c r="I130" s="19"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131" s="20"/>
       <c r="B131" s="19"/>
       <c r="C131" s="19"/>
@@ -4197,7 +4222,7 @@
       <c r="H131" s="19"/>
       <c r="I131" s="19"/>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132" s="20"/>
       <c r="B132" s="19"/>
       <c r="C132" s="19"/>
@@ -4208,7 +4233,7 @@
       <c r="H132" s="19"/>
       <c r="I132" s="19"/>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133" s="20"/>
       <c r="B133" s="19"/>
       <c r="C133" s="19"/>
@@ -4219,7 +4244,7 @@
       <c r="H133" s="19"/>
       <c r="I133" s="19"/>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134" s="20"/>
       <c r="B134" s="19"/>
       <c r="C134" s="19"/>
@@ -4230,7 +4255,7 @@
       <c r="H134" s="19"/>
       <c r="I134" s="19"/>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" s="20"/>
       <c r="B135" s="19"/>
       <c r="C135" s="19"/>
@@ -4241,7 +4266,7 @@
       <c r="H135" s="19"/>
       <c r="I135" s="19"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136" s="20"/>
       <c r="B136" s="19"/>
       <c r="C136" s="19"/>
@@ -4252,7 +4277,7 @@
       <c r="H136" s="19"/>
       <c r="I136" s="19"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137" s="20"/>
       <c r="B137" s="19"/>
       <c r="C137" s="19"/>
@@ -4263,7 +4288,7 @@
       <c r="H137" s="19"/>
       <c r="I137" s="19"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" s="20"/>
       <c r="B138" s="19"/>
       <c r="C138" s="19"/>
@@ -4274,7 +4299,7 @@
       <c r="H138" s="19"/>
       <c r="I138" s="19"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139" s="20"/>
       <c r="B139" s="19"/>
       <c r="C139" s="19"/>
@@ -4285,7 +4310,7 @@
       <c r="H139" s="19"/>
       <c r="I139" s="19"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140" s="20"/>
       <c r="B140" s="19"/>
       <c r="C140" s="19"/>
@@ -4296,7 +4321,7 @@
       <c r="H140" s="19"/>
       <c r="I140" s="19"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A141" s="20"/>
       <c r="B141" s="19"/>
       <c r="C141" s="19"/>
@@ -4307,7 +4332,7 @@
       <c r="H141" s="19"/>
       <c r="I141" s="19"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A142" s="20"/>
       <c r="B142" s="19"/>
       <c r="C142" s="19"/>
@@ -4318,7 +4343,7 @@
       <c r="H142" s="19"/>
       <c r="I142" s="19"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A143" s="20"/>
       <c r="B143" s="19"/>
       <c r="C143" s="19"/>
@@ -4329,7 +4354,7 @@
       <c r="H143" s="19"/>
       <c r="I143" s="19"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144" s="20"/>
       <c r="B144" s="19"/>
       <c r="C144" s="19"/>
@@ -4340,7 +4365,7 @@
       <c r="H144" s="19"/>
       <c r="I144" s="19"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" s="20"/>
       <c r="B145" s="19"/>
       <c r="C145" s="19"/>
@@ -4351,7 +4376,7 @@
       <c r="H145" s="19"/>
       <c r="I145" s="19"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" s="20"/>
       <c r="B146" s="19"/>
       <c r="C146" s="19"/>
@@ -4362,7 +4387,7 @@
       <c r="H146" s="19"/>
       <c r="I146" s="19"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147" s="20"/>
       <c r="B147" s="19"/>
       <c r="C147" s="19"/>
@@ -4373,7 +4398,7 @@
       <c r="H147" s="19"/>
       <c r="I147" s="19"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" s="20"/>
       <c r="B148" s="19"/>
       <c r="C148" s="19"/>
@@ -4384,7 +4409,7 @@
       <c r="H148" s="19"/>
       <c r="I148" s="19"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149" s="20"/>
       <c r="B149" s="19"/>
       <c r="C149" s="19"/>
@@ -4395,7 +4420,7 @@
       <c r="H149" s="19"/>
       <c r="I149" s="19"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150" s="20"/>
       <c r="B150" s="19"/>
       <c r="C150" s="19"/>
@@ -4406,7 +4431,7 @@
       <c r="H150" s="19"/>
       <c r="I150" s="19"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151" s="20"/>
       <c r="B151" s="19"/>
       <c r="C151" s="19"/>
@@ -4417,7 +4442,7 @@
       <c r="H151" s="19"/>
       <c r="I151" s="19"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152" s="20"/>
       <c r="B152" s="19"/>
       <c r="C152" s="19"/>
@@ -4428,7 +4453,7 @@
       <c r="H152" s="19"/>
       <c r="I152" s="19"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153" s="20"/>
       <c r="B153" s="19"/>
       <c r="C153" s="19"/>
@@ -4439,7 +4464,7 @@
       <c r="H153" s="19"/>
       <c r="I153" s="19"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A154" s="20"/>
       <c r="B154" s="19"/>
       <c r="C154" s="19"/>
@@ -4450,7 +4475,7 @@
       <c r="H154" s="19"/>
       <c r="I154" s="19"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155" s="20"/>
       <c r="B155" s="19"/>
       <c r="C155" s="19"/>
@@ -4461,7 +4486,7 @@
       <c r="H155" s="19"/>
       <c r="I155" s="19"/>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A156" s="20"/>
       <c r="B156" s="19"/>
       <c r="C156" s="19"/>
@@ -4472,7 +4497,7 @@
       <c r="H156" s="19"/>
       <c r="I156" s="19"/>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A157" s="20"/>
       <c r="B157" s="19"/>
       <c r="C157" s="19"/>
@@ -4483,7 +4508,7 @@
       <c r="H157" s="19"/>
       <c r="I157" s="19"/>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A158" s="20"/>
       <c r="B158" s="19"/>
       <c r="C158" s="19"/>
@@ -4494,7 +4519,7 @@
       <c r="H158" s="19"/>
       <c r="I158" s="19"/>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A159" s="20"/>
       <c r="B159" s="19"/>
       <c r="C159" s="19"/>
@@ -4505,7 +4530,7 @@
       <c r="H159" s="19"/>
       <c r="I159" s="19"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A160" s="20"/>
       <c r="B160" s="19"/>
       <c r="C160" s="19"/>
@@ -4516,7 +4541,7 @@
       <c r="H160" s="19"/>
       <c r="I160" s="19"/>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161" s="20"/>
       <c r="B161" s="19"/>
       <c r="C161" s="19"/>
@@ -4527,7 +4552,7 @@
       <c r="H161" s="19"/>
       <c r="I161" s="19"/>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A162" s="20"/>
       <c r="B162" s="19"/>
       <c r="C162" s="19"/>
@@ -4538,7 +4563,7 @@
       <c r="H162" s="19"/>
       <c r="I162" s="19"/>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A163" s="20"/>
       <c r="B163" s="19"/>
       <c r="C163" s="19"/>
@@ -4549,7 +4574,7 @@
       <c r="H163" s="19"/>
       <c r="I163" s="19"/>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A164" s="20"/>
       <c r="B164" s="19"/>
       <c r="C164" s="19"/>
@@ -4560,7 +4585,7 @@
       <c r="H164" s="19"/>
       <c r="I164" s="19"/>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A165" s="20"/>
       <c r="B165" s="19"/>
       <c r="C165" s="19"/>
@@ -4571,7 +4596,7 @@
       <c r="H165" s="19"/>
       <c r="I165" s="19"/>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A166" s="20"/>
       <c r="B166" s="19"/>
       <c r="C166" s="19"/>
@@ -4582,7 +4607,7 @@
       <c r="H166" s="19"/>
       <c r="I166" s="19"/>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A167" s="20"/>
       <c r="B167" s="19"/>
       <c r="C167" s="19"/>
@@ -4593,7 +4618,7 @@
       <c r="H167" s="19"/>
       <c r="I167" s="19"/>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A168" s="20"/>
       <c r="B168" s="19"/>
       <c r="C168" s="19"/>
@@ -4604,7 +4629,7 @@
       <c r="H168" s="19"/>
       <c r="I168" s="19"/>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A169" s="20"/>
       <c r="B169" s="19"/>
       <c r="C169" s="19"/>
@@ -4615,7 +4640,7 @@
       <c r="H169" s="19"/>
       <c r="I169" s="19"/>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A170" s="20"/>
       <c r="B170" s="19"/>
       <c r="C170" s="19"/>
@@ -4626,7 +4651,7 @@
       <c r="H170" s="19"/>
       <c r="I170" s="19"/>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A171" s="20"/>
       <c r="B171" s="19"/>
       <c r="C171" s="19"/>
@@ -4637,7 +4662,7 @@
       <c r="H171" s="19"/>
       <c r="I171" s="19"/>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A172" s="20"/>
       <c r="B172" s="19"/>
       <c r="C172" s="19"/>
@@ -4648,7 +4673,7 @@
       <c r="H172" s="19"/>
       <c r="I172" s="19"/>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A173" s="20"/>
       <c r="B173" s="19"/>
       <c r="C173" s="19"/>
@@ -4659,7 +4684,7 @@
       <c r="H173" s="19"/>
       <c r="I173" s="19"/>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A174" s="20"/>
       <c r="B174" s="19"/>
       <c r="C174" s="19"/>
@@ -4670,7 +4695,7 @@
       <c r="H174" s="19"/>
       <c r="I174" s="19"/>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A175" s="20"/>
       <c r="B175" s="19"/>
       <c r="C175" s="19"/>
@@ -4681,7 +4706,7 @@
       <c r="H175" s="19"/>
       <c r="I175" s="19"/>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A176" s="20"/>
       <c r="B176" s="19"/>
       <c r="C176" s="19"/>
@@ -4692,7 +4717,7 @@
       <c r="H176" s="19"/>
       <c r="I176" s="19"/>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A177" s="20"/>
       <c r="B177" s="19"/>
       <c r="C177" s="19"/>
@@ -4703,7 +4728,7 @@
       <c r="H177" s="19"/>
       <c r="I177" s="19"/>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A178" s="20"/>
       <c r="B178" s="19"/>
       <c r="C178" s="19"/>
@@ -4714,7 +4739,7 @@
       <c r="H178" s="19"/>
       <c r="I178" s="19"/>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A179" s="20"/>
       <c r="B179" s="19"/>
       <c r="C179" s="19"/>
@@ -4725,7 +4750,7 @@
       <c r="H179" s="19"/>
       <c r="I179" s="19"/>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A180" s="20"/>
       <c r="B180" s="19"/>
       <c r="C180" s="19"/>
@@ -4736,7 +4761,7 @@
       <c r="H180" s="19"/>
       <c r="I180" s="19"/>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A181" s="20"/>
       <c r="B181" s="19"/>
       <c r="C181" s="19"/>
@@ -4747,7 +4772,7 @@
       <c r="H181" s="19"/>
       <c r="I181" s="19"/>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A182" s="20"/>
       <c r="B182" s="19"/>
       <c r="C182" s="19"/>
@@ -4758,7 +4783,7 @@
       <c r="H182" s="19"/>
       <c r="I182" s="19"/>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A183" s="20"/>
       <c r="B183" s="19"/>
       <c r="C183" s="19"/>
@@ -4769,7 +4794,7 @@
       <c r="H183" s="19"/>
       <c r="I183" s="19"/>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A184" s="20"/>
       <c r="B184" s="19"/>
       <c r="C184" s="19"/>
@@ -4780,7 +4805,7 @@
       <c r="H184" s="19"/>
       <c r="I184" s="19"/>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A185" s="20"/>
       <c r="B185" s="19"/>
       <c r="C185" s="19"/>
@@ -4791,7 +4816,7 @@
       <c r="H185" s="19"/>
       <c r="I185" s="19"/>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A186" s="20"/>
       <c r="B186" s="19"/>
       <c r="C186" s="19"/>
@@ -4802,7 +4827,7 @@
       <c r="H186" s="19"/>
       <c r="I186" s="19"/>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A187" s="20"/>
       <c r="B187" s="19"/>
       <c r="C187" s="19"/>
@@ -4813,7 +4838,7 @@
       <c r="H187" s="19"/>
       <c r="I187" s="19"/>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A188" s="20"/>
       <c r="B188" s="19"/>
       <c r="C188" s="19"/>
@@ -4824,7 +4849,7 @@
       <c r="H188" s="19"/>
       <c r="I188" s="19"/>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A189" s="20"/>
       <c r="B189" s="19"/>
       <c r="C189" s="19"/>
@@ -4835,7 +4860,7 @@
       <c r="H189" s="19"/>
       <c r="I189" s="19"/>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A190" s="20"/>
       <c r="B190" s="19"/>
       <c r="C190" s="19"/>
@@ -4846,7 +4871,7 @@
       <c r="H190" s="19"/>
       <c r="I190" s="19"/>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A191" s="20"/>
       <c r="B191" s="19"/>
       <c r="C191" s="19"/>
@@ -4857,7 +4882,7 @@
       <c r="H191" s="19"/>
       <c r="I191" s="19"/>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A192" s="20"/>
       <c r="B192" s="19"/>
       <c r="C192" s="19"/>
@@ -4868,7 +4893,7 @@
       <c r="H192" s="19"/>
       <c r="I192" s="19"/>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A193" s="20"/>
       <c r="B193" s="19"/>
       <c r="C193" s="19"/>
@@ -4879,7 +4904,7 @@
       <c r="H193" s="19"/>
       <c r="I193" s="19"/>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A194" s="20"/>
       <c r="B194" s="19"/>
       <c r="C194" s="19"/>
@@ -4890,7 +4915,7 @@
       <c r="H194" s="19"/>
       <c r="I194" s="19"/>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A195" s="20"/>
       <c r="B195" s="19"/>
       <c r="C195" s="19"/>
@@ -4901,7 +4926,7 @@
       <c r="H195" s="19"/>
       <c r="I195" s="19"/>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A196" s="20"/>
       <c r="B196" s="19"/>
       <c r="C196" s="19"/>
@@ -4912,7 +4937,7 @@
       <c r="H196" s="19"/>
       <c r="I196" s="19"/>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A197" s="20"/>
       <c r="B197" s="19"/>
       <c r="C197" s="19"/>
@@ -4923,7 +4948,7 @@
       <c r="H197" s="19"/>
       <c r="I197" s="19"/>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A198" s="20"/>
       <c r="B198" s="19"/>
       <c r="C198" s="19"/>
@@ -4934,7 +4959,7 @@
       <c r="H198" s="19"/>
       <c r="I198" s="19"/>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A199" s="20"/>
       <c r="B199" s="19"/>
       <c r="C199" s="19"/>
@@ -4945,7 +4970,7 @@
       <c r="H199" s="19"/>
       <c r="I199" s="19"/>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A200" s="20"/>
       <c r="B200" s="19"/>
       <c r="C200" s="19"/>
@@ -4956,7 +4981,7 @@
       <c r="H200" s="19"/>
       <c r="I200" s="19"/>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A201" s="20"/>
       <c r="B201" s="19"/>
       <c r="C201" s="19"/>
@@ -4967,7 +4992,7 @@
       <c r="H201" s="19"/>
       <c r="I201" s="19"/>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A202" s="20"/>
       <c r="B202" s="19"/>
       <c r="C202" s="19"/>
@@ -4978,7 +5003,7 @@
       <c r="H202" s="19"/>
       <c r="I202" s="19"/>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A203" s="20"/>
       <c r="B203" s="19"/>
       <c r="C203" s="19"/>
@@ -4989,7 +5014,7 @@
       <c r="H203" s="19"/>
       <c r="I203" s="19"/>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A204" s="20"/>
       <c r="B204" s="19"/>
       <c r="C204" s="19"/>
@@ -5000,7 +5025,7 @@
       <c r="H204" s="19"/>
       <c r="I204" s="19"/>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A205" s="20"/>
       <c r="B205" s="19"/>
       <c r="C205" s="19"/>
@@ -5011,7 +5036,7 @@
       <c r="H205" s="19"/>
       <c r="I205" s="19"/>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A206" s="20"/>
       <c r="B206" s="19"/>
       <c r="C206" s="19"/>
@@ -5022,7 +5047,7 @@
       <c r="H206" s="19"/>
       <c r="I206" s="19"/>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A207" s="20"/>
       <c r="B207" s="19"/>
       <c r="C207" s="19"/>
@@ -5033,7 +5058,7 @@
       <c r="H207" s="19"/>
       <c r="I207" s="19"/>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A208" s="20"/>
       <c r="B208" s="19"/>
       <c r="C208" s="19"/>
@@ -5044,7 +5069,7 @@
       <c r="H208" s="19"/>
       <c r="I208" s="19"/>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A209" s="20"/>
       <c r="B209" s="19"/>
       <c r="C209" s="19"/>
@@ -5055,7 +5080,7 @@
       <c r="H209" s="19"/>
       <c r="I209" s="19"/>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A210" s="20"/>
       <c r="B210" s="19"/>
       <c r="C210" s="19"/>
@@ -5066,7 +5091,7 @@
       <c r="H210" s="19"/>
       <c r="I210" s="19"/>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A211" s="20"/>
       <c r="B211" s="19"/>
       <c r="C211" s="19"/>
@@ -5077,7 +5102,7 @@
       <c r="H211" s="19"/>
       <c r="I211" s="19"/>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A212" s="20"/>
       <c r="B212" s="19"/>
       <c r="C212" s="19"/>
@@ -5088,7 +5113,7 @@
       <c r="H212" s="19"/>
       <c r="I212" s="19"/>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A213" s="20"/>
       <c r="B213" s="19"/>
       <c r="C213" s="19"/>
@@ -5099,7 +5124,7 @@
       <c r="H213" s="19"/>
       <c r="I213" s="19"/>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A214" s="20"/>
       <c r="B214" s="19"/>
       <c r="C214" s="19"/>
@@ -5110,7 +5135,7 @@
       <c r="H214" s="19"/>
       <c r="I214" s="19"/>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A215" s="20"/>
       <c r="B215" s="19"/>
       <c r="C215" s="19"/>
@@ -5121,7 +5146,7 @@
       <c r="H215" s="19"/>
       <c r="I215" s="19"/>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A216" s="20"/>
       <c r="B216" s="19"/>
       <c r="C216" s="19"/>
@@ -5132,7 +5157,7 @@
       <c r="H216" s="19"/>
       <c r="I216" s="19"/>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A217" s="20"/>
       <c r="B217" s="19"/>
       <c r="C217" s="19"/>
@@ -5143,7 +5168,7 @@
       <c r="H217" s="19"/>
       <c r="I217" s="19"/>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A218" s="20"/>
       <c r="B218" s="19"/>
       <c r="C218" s="19"/>
@@ -5154,7 +5179,7 @@
       <c r="H218" s="19"/>
       <c r="I218" s="19"/>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A219" s="20"/>
       <c r="B219" s="19"/>
       <c r="C219" s="19"/>
@@ -5165,7 +5190,7 @@
       <c r="H219" s="19"/>
       <c r="I219" s="19"/>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A220" s="20"/>
       <c r="B220" s="19"/>
       <c r="C220" s="19"/>
@@ -5176,7 +5201,7 @@
       <c r="H220" s="19"/>
       <c r="I220" s="19"/>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A221" s="20"/>
       <c r="B221" s="19"/>
       <c r="C221" s="19"/>
@@ -5187,7 +5212,7 @@
       <c r="H221" s="19"/>
       <c r="I221" s="19"/>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A222" s="20"/>
       <c r="B222" s="19"/>
       <c r="C222" s="19"/>
@@ -5198,7 +5223,7 @@
       <c r="H222" s="19"/>
       <c r="I222" s="19"/>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A223" s="20"/>
       <c r="B223" s="19"/>
       <c r="C223" s="19"/>
@@ -5209,7 +5234,7 @@
       <c r="H223" s="19"/>
       <c r="I223" s="19"/>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A224" s="20"/>
       <c r="B224" s="19"/>
       <c r="C224" s="19"/>
@@ -5220,7 +5245,7 @@
       <c r="H224" s="19"/>
       <c r="I224" s="19"/>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A225" s="20"/>
       <c r="B225" s="19"/>
       <c r="C225" s="19"/>
@@ -5231,7 +5256,7 @@
       <c r="H225" s="19"/>
       <c r="I225" s="19"/>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A226" s="20"/>
       <c r="B226" s="19"/>
       <c r="C226" s="19"/>
@@ -5242,7 +5267,7 @@
       <c r="H226" s="19"/>
       <c r="I226" s="19"/>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A227" s="20"/>
       <c r="B227" s="19"/>
       <c r="C227" s="19"/>
@@ -5253,7 +5278,7 @@
       <c r="H227" s="19"/>
       <c r="I227" s="19"/>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A228" s="20"/>
       <c r="B228" s="19"/>
       <c r="C228" s="19"/>
@@ -5264,7 +5289,7 @@
       <c r="H228" s="19"/>
       <c r="I228" s="19"/>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A229" s="20"/>
       <c r="B229" s="19"/>
       <c r="C229" s="19"/>
@@ -5275,7 +5300,7 @@
       <c r="H229" s="19"/>
       <c r="I229" s="19"/>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A230" s="20"/>
       <c r="B230" s="19"/>
       <c r="C230" s="19"/>
@@ -5286,7 +5311,7 @@
       <c r="H230" s="19"/>
       <c r="I230" s="19"/>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A231" s="20"/>
       <c r="B231" s="19"/>
       <c r="C231" s="19"/>
@@ -5297,7 +5322,7 @@
       <c r="H231" s="19"/>
       <c r="I231" s="19"/>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A232" s="20"/>
       <c r="B232" s="19"/>
       <c r="C232" s="19"/>
@@ -5308,7 +5333,7 @@
       <c r="H232" s="19"/>
       <c r="I232" s="19"/>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A233" s="20"/>
       <c r="B233" s="19"/>
       <c r="C233" s="19"/>
@@ -5319,7 +5344,7 @@
       <c r="H233" s="19"/>
       <c r="I233" s="19"/>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A234" s="20"/>
       <c r="B234" s="19"/>
       <c r="C234" s="19"/>
@@ -5330,7 +5355,7 @@
       <c r="H234" s="19"/>
       <c r="I234" s="19"/>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A235" s="20"/>
       <c r="B235" s="19"/>
       <c r="C235" s="19"/>
@@ -5341,7 +5366,7 @@
       <c r="H235" s="19"/>
       <c r="I235" s="19"/>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A236" s="20"/>
       <c r="B236" s="19"/>
       <c r="C236" s="19"/>
@@ -5352,7 +5377,7 @@
       <c r="H236" s="19"/>
       <c r="I236" s="19"/>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A237" s="20"/>
       <c r="B237" s="19"/>
       <c r="C237" s="19"/>
@@ -5363,7 +5388,7 @@
       <c r="H237" s="19"/>
       <c r="I237" s="19"/>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A238" s="20"/>
       <c r="B238" s="19"/>
       <c r="C238" s="19"/>
@@ -5374,7 +5399,7 @@
       <c r="H238" s="19"/>
       <c r="I238" s="19"/>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A239" s="20"/>
       <c r="B239" s="19"/>
       <c r="C239" s="19"/>
@@ -5385,7 +5410,7 @@
       <c r="H239" s="19"/>
       <c r="I239" s="19"/>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A240" s="20"/>
       <c r="B240" s="19"/>
       <c r="C240" s="19"/>
@@ -5396,7 +5421,7 @@
       <c r="H240" s="19"/>
       <c r="I240" s="19"/>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A241" s="20"/>
       <c r="B241" s="19"/>
       <c r="C241" s="19"/>
@@ -5407,7 +5432,7 @@
       <c r="H241" s="19"/>
       <c r="I241" s="19"/>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A242" s="20"/>
       <c r="B242" s="19"/>
       <c r="C242" s="19"/>
@@ -5418,7 +5443,7 @@
       <c r="H242" s="19"/>
       <c r="I242" s="19"/>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A243" s="20"/>
       <c r="B243" s="19"/>
       <c r="C243" s="19"/>
@@ -5429,7 +5454,7 @@
       <c r="H243" s="19"/>
       <c r="I243" s="19"/>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A244" s="20"/>
       <c r="B244" s="19"/>
       <c r="C244" s="19"/>
@@ -5440,7 +5465,7 @@
       <c r="H244" s="19"/>
       <c r="I244" s="19"/>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A245" s="20"/>
       <c r="B245" s="19"/>
       <c r="C245" s="19"/>
@@ -5451,7 +5476,7 @@
       <c r="H245" s="19"/>
       <c r="I245" s="19"/>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A246" s="20"/>
       <c r="B246" s="19"/>
       <c r="C246" s="19"/>
@@ -5462,7 +5487,7 @@
       <c r="H246" s="19"/>
       <c r="I246" s="19"/>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A247" s="20"/>
       <c r="B247" s="19"/>
       <c r="C247" s="19"/>
@@ -5473,7 +5498,7 @@
       <c r="H247" s="19"/>
       <c r="I247" s="19"/>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A248" s="20"/>
       <c r="B248" s="19"/>
       <c r="C248" s="19"/>
@@ -5484,7 +5509,7 @@
       <c r="H248" s="19"/>
       <c r="I248" s="19"/>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A249" s="20"/>
       <c r="B249" s="19"/>
       <c r="C249" s="19"/>
@@ -5495,7 +5520,7 @@
       <c r="H249" s="19"/>
       <c r="I249" s="19"/>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A250" s="20"/>
       <c r="B250" s="19"/>
       <c r="C250" s="19"/>
@@ -5506,7 +5531,7 @@
       <c r="H250" s="19"/>
       <c r="I250" s="19"/>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A251" s="20"/>
       <c r="B251" s="19"/>
       <c r="C251" s="19"/>
@@ -5517,7 +5542,7 @@
       <c r="H251" s="19"/>
       <c r="I251" s="19"/>
     </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A252" s="20"/>
       <c r="B252" s="19"/>
       <c r="C252" s="19"/>
@@ -5528,7 +5553,7 @@
       <c r="H252" s="19"/>
       <c r="I252" s="19"/>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A253" s="20"/>
       <c r="B253" s="19"/>
       <c r="C253" s="19"/>
@@ -5539,7 +5564,7 @@
       <c r="H253" s="19"/>
       <c r="I253" s="19"/>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A254" s="20"/>
       <c r="B254" s="19"/>
       <c r="C254" s="19"/>
@@ -5550,7 +5575,7 @@
       <c r="H254" s="19"/>
       <c r="I254" s="19"/>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A255" s="20"/>
       <c r="B255" s="19"/>
       <c r="C255" s="19"/>
@@ -5561,7 +5586,7 @@
       <c r="H255" s="19"/>
       <c r="I255" s="19"/>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A256" s="20"/>
       <c r="B256" s="19"/>
       <c r="C256" s="19"/>
@@ -5572,7 +5597,7 @@
       <c r="H256" s="19"/>
       <c r="I256" s="19"/>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A257" s="20"/>
       <c r="B257" s="19"/>
       <c r="C257" s="19"/>
@@ -5583,7 +5608,7 @@
       <c r="H257" s="19"/>
       <c r="I257" s="19"/>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A258" s="20"/>
       <c r="B258" s="19"/>
       <c r="C258" s="19"/>
@@ -5594,7 +5619,7 @@
       <c r="H258" s="19"/>
       <c r="I258" s="19"/>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A259" s="20"/>
       <c r="B259" s="19"/>
       <c r="C259" s="19"/>
@@ -5605,7 +5630,7 @@
       <c r="H259" s="19"/>
       <c r="I259" s="19"/>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A260" s="20"/>
       <c r="B260" s="19"/>
       <c r="C260" s="19"/>
@@ -5616,7 +5641,7 @@
       <c r="H260" s="19"/>
       <c r="I260" s="19"/>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A261" s="20"/>
       <c r="B261" s="19"/>
       <c r="C261" s="19"/>
@@ -5627,7 +5652,7 @@
       <c r="H261" s="19"/>
       <c r="I261" s="19"/>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A262" s="20"/>
       <c r="B262" s="19"/>
       <c r="C262" s="19"/>
@@ -5638,7 +5663,7 @@
       <c r="H262" s="19"/>
       <c r="I262" s="19"/>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A263" s="20"/>
       <c r="B263" s="19"/>
       <c r="C263" s="19"/>
@@ -5649,7 +5674,7 @@
       <c r="H263" s="19"/>
       <c r="I263" s="19"/>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A264" s="20"/>
       <c r="B264" s="19"/>
       <c r="C264" s="19"/>
@@ -5660,7 +5685,7 @@
       <c r="H264" s="19"/>
       <c r="I264" s="19"/>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A265" s="20"/>
       <c r="B265" s="19"/>
       <c r="C265" s="19"/>
@@ -5671,7 +5696,7 @@
       <c r="H265" s="19"/>
       <c r="I265" s="19"/>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A266" s="20"/>
       <c r="B266" s="19"/>
       <c r="C266" s="19"/>
@@ -5682,7 +5707,7 @@
       <c r="H266" s="19"/>
       <c r="I266" s="19"/>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A267" s="20"/>
       <c r="B267" s="19"/>
       <c r="C267" s="19"/>
@@ -5693,7 +5718,7 @@
       <c r="H267" s="19"/>
       <c r="I267" s="19"/>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A268" s="20"/>
       <c r="B268" s="19"/>
       <c r="C268" s="19"/>
@@ -5704,7 +5729,7 @@
       <c r="H268" s="19"/>
       <c r="I268" s="19"/>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A269" s="20"/>
       <c r="B269" s="19"/>
       <c r="C269" s="19"/>
@@ -5715,7 +5740,7 @@
       <c r="H269" s="19"/>
       <c r="I269" s="19"/>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A270" s="20"/>
       <c r="B270" s="19"/>
       <c r="C270" s="19"/>
@@ -5726,7 +5751,7 @@
       <c r="H270" s="19"/>
       <c r="I270" s="19"/>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A271" s="20"/>
       <c r="B271" s="19"/>
       <c r="C271" s="19"/>
@@ -5737,7 +5762,7 @@
       <c r="H271" s="19"/>
       <c r="I271" s="19"/>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A272" s="20"/>
       <c r="B272" s="19"/>
       <c r="C272" s="19"/>
@@ -5748,7 +5773,7 @@
       <c r="H272" s="19"/>
       <c r="I272" s="19"/>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A273" s="20"/>
       <c r="B273" s="19"/>
       <c r="C273" s="19"/>
@@ -5759,7 +5784,7 @@
       <c r="H273" s="19"/>
       <c r="I273" s="19"/>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A274" s="20"/>
       <c r="B274" s="19"/>
       <c r="C274" s="19"/>
@@ -5770,7 +5795,7 @@
       <c r="H274" s="19"/>
       <c r="I274" s="19"/>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A275" s="20"/>
       <c r="B275" s="19"/>
       <c r="C275" s="19"/>
@@ -5781,7 +5806,7 @@
       <c r="H275" s="19"/>
       <c r="I275" s="19"/>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A276" s="20"/>
       <c r="B276" s="19"/>
       <c r="C276" s="19"/>
@@ -5792,7 +5817,7 @@
       <c r="H276" s="19"/>
       <c r="I276" s="19"/>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A277" s="20"/>
       <c r="B277" s="19"/>
       <c r="C277" s="19"/>
@@ -5803,7 +5828,7 @@
       <c r="H277" s="19"/>
       <c r="I277" s="19"/>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A278" s="20"/>
       <c r="B278" s="19"/>
       <c r="C278" s="19"/>
@@ -5814,7 +5839,7 @@
       <c r="H278" s="19"/>
       <c r="I278" s="19"/>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A279" s="20"/>
       <c r="B279" s="19"/>
       <c r="C279" s="19"/>
@@ -5825,7 +5850,7 @@
       <c r="H279" s="19"/>
       <c r="I279" s="19"/>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A280" s="20"/>
       <c r="B280" s="19"/>
       <c r="C280" s="19"/>
@@ -5836,7 +5861,7 @@
       <c r="H280" s="19"/>
       <c r="I280" s="19"/>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A281" s="20"/>
       <c r="B281" s="19"/>
       <c r="C281" s="19"/>
@@ -5847,7 +5872,7 @@
       <c r="H281" s="22"/>
       <c r="I281" s="22"/>
     </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A282" s="20"/>
       <c r="B282" s="19"/>
       <c r="C282" s="19"/>
@@ -5856,7 +5881,7 @@
       <c r="F282" s="23"/>
       <c r="G282" s="23"/>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A283" s="20"/>
       <c r="B283" s="19"/>
       <c r="C283" s="19"/>
@@ -5865,7 +5890,7 @@
       <c r="F283" s="23"/>
       <c r="G283" s="23"/>
     </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A284" s="20"/>
       <c r="B284" s="19"/>
       <c r="C284" s="19"/>
@@ -5874,7 +5899,7 @@
       <c r="F284" s="23"/>
       <c r="G284" s="23"/>
     </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A285" s="20"/>
       <c r="B285" s="19"/>
       <c r="C285" s="19"/>
@@ -5883,7 +5908,7 @@
       <c r="F285" s="23"/>
       <c r="G285" s="23"/>
     </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A286" s="20"/>
       <c r="B286" s="19"/>
       <c r="C286" s="19"/>
@@ -5892,7 +5917,7 @@
       <c r="F286" s="23"/>
       <c r="G286" s="23"/>
     </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A287" s="20"/>
       <c r="B287" s="19"/>
       <c r="C287" s="19"/>
@@ -5901,7 +5926,7 @@
       <c r="F287" s="23"/>
       <c r="G287" s="23"/>
     </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A288" s="20"/>
       <c r="B288" s="19"/>
       <c r="C288" s="19"/>
@@ -5910,7 +5935,7 @@
       <c r="F288" s="23"/>
       <c r="G288" s="23"/>
     </row>
-    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A289" s="20"/>
       <c r="B289" s="19"/>
       <c r="C289" s="19"/>
@@ -5919,7 +5944,7 @@
       <c r="F289" s="23"/>
       <c r="G289" s="23"/>
     </row>
-    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A290" s="20"/>
       <c r="B290" s="19"/>
       <c r="C290" s="19"/>
@@ -5928,7 +5953,7 @@
       <c r="F290" s="23"/>
       <c r="G290" s="23"/>
     </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A291" s="20"/>
       <c r="B291" s="19"/>
       <c r="C291" s="19"/>
@@ -5937,7 +5962,7 @@
       <c r="F291" s="23"/>
       <c r="G291" s="23"/>
     </row>
-    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A292" s="20"/>
       <c r="B292" s="19"/>
       <c r="C292" s="19"/>
@@ -5946,7 +5971,7 @@
       <c r="F292" s="23"/>
       <c r="G292" s="23"/>
     </row>
-    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A293" s="20"/>
       <c r="B293" s="19"/>
       <c r="C293" s="19"/>
@@ -5955,7 +5980,7 @@
       <c r="F293" s="23"/>
       <c r="G293" s="23"/>
     </row>
-    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A294" s="20"/>
       <c r="B294" s="19"/>
       <c r="C294" s="19"/>
@@ -5964,7 +5989,7 @@
       <c r="F294" s="23"/>
       <c r="G294" s="23"/>
     </row>
-    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A295" s="20"/>
       <c r="B295" s="19"/>
       <c r="C295" s="19"/>
@@ -5973,7 +5998,7 @@
       <c r="F295" s="23"/>
       <c r="G295" s="23"/>
     </row>
-    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A296" s="20"/>
       <c r="B296" s="19"/>
       <c r="C296" s="19"/>
@@ -5982,7 +6007,7 @@
       <c r="F296" s="23"/>
       <c r="G296" s="23"/>
     </row>
-    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A297" s="20"/>
       <c r="B297" s="19"/>
       <c r="C297" s="19"/>
@@ -5991,7 +6016,7 @@
       <c r="F297" s="23"/>
       <c r="G297" s="23"/>
     </row>
-    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A298" s="20"/>
       <c r="B298" s="19"/>
       <c r="C298" s="19"/>
@@ -6000,7 +6025,7 @@
       <c r="F298" s="23"/>
       <c r="G298" s="23"/>
     </row>
-    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A299" s="20"/>
       <c r="B299" s="19"/>
       <c r="C299" s="19"/>
@@ -6009,7 +6034,7 @@
       <c r="F299" s="23"/>
       <c r="G299" s="23"/>
     </row>
-    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A300" s="20"/>
       <c r="B300" s="19"/>
       <c r="C300" s="19"/>
@@ -6018,7 +6043,7 @@
       <c r="F300" s="23"/>
       <c r="G300" s="23"/>
     </row>
-    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A301" s="20"/>
       <c r="B301" s="19"/>
       <c r="C301" s="19"/>
@@ -6027,7 +6052,7 @@
       <c r="F301" s="23"/>
       <c r="G301" s="23"/>
     </row>
-    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A302" s="20"/>
       <c r="B302" s="19"/>
       <c r="C302" s="19"/>
@@ -6036,7 +6061,7 @@
       <c r="F302" s="23"/>
       <c r="G302" s="23"/>
     </row>
-    <row r="303" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A303" s="20"/>
       <c r="B303" s="19"/>
       <c r="C303" s="19"/>
@@ -6045,7 +6070,7 @@
       <c r="F303" s="23"/>
       <c r="G303" s="23"/>
     </row>
-    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A304" s="20"/>
       <c r="B304" s="19"/>
       <c r="C304" s="22"/>
@@ -6054,7 +6079,7 @@
       <c r="F304" s="23"/>
       <c r="G304" s="23"/>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A305" s="21"/>
       <c r="B305" s="22"/>
     </row>
@@ -6070,11 +6095,11 @@
     <mergeCell ref="F2:G2"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A64 A71:A515">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A64 A71:A515" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>43831</formula1>
       <formula2>44561</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I299 H63:H299 H5:H60 B5:B64 B71:B323 C5:C322">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I299 H63:H299 H5:H60 B5:B64 B71:B323 C5:C322" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>0</formula1>
       <formula2>10000000</formula2>
     </dataValidation>
@@ -6084,41 +6109,41 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="14.375" customWidth="1"/>
-    <col min="4" max="4" width="16.125" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C4" s="45" t="s">
         <v>79</v>
       </c>
       <c r="D4" s="46"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="30" t="s">
         <v>12</v>
       </c>
@@ -6132,7 +6157,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="30" t="s">
         <v>75</v>
       </c>
@@ -6146,7 +6171,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="30" t="s">
         <v>76</v>
       </c>
@@ -6160,7 +6185,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="30" t="s">
         <v>77</v>
       </c>
@@ -6174,7 +6199,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="s">
         <v>78</v>
       </c>
@@ -6188,16 +6213,16 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C4:D4"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:D9">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:D9" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>0</formula1>
       <formula2>20</formula2>
     </dataValidation>
@@ -6207,21 +6232,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.125" customWidth="1"/>
+    <col min="1" max="1" width="25.1640625" customWidth="1"/>
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.875" style="1"/>
+    <col min="3" max="3" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -6235,7 +6260,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>15</v>
       </c>
@@ -6246,7 +6271,7 @@
         <v>12345</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>16</v>
       </c>
@@ -6260,7 +6285,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>18</v>
       </c>
@@ -6274,7 +6299,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>17</v>
       </c>
@@ -6285,7 +6310,7 @@
         <v>43877</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>23</v>
       </c>
@@ -6299,7 +6324,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>24</v>
       </c>
@@ -6313,7 +6338,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>37</v>
       </c>
@@ -6327,7 +6352,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
         <v>38</v>
       </c>
@@ -6339,7 +6364,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
         <v>39</v>
       </c>
@@ -6350,7 +6375,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
         <v>40</v>
       </c>
@@ -6364,7 +6389,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
         <v>41</v>
       </c>
@@ -6378,7 +6403,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>82</v>
       </c>
@@ -6391,15 +6416,15 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>1</formula1>
       <formula2>10000000</formula2>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>43831</formula1>
       <formula2>44561</formula2>
     </dataValidation>
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="B4 B6:B7">
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="B4 B6:B7" xr:uid="{00000000-0002-0000-0500-000002000000}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
update Riverside and SF
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43792D3-8633-ED4B-B99A-8E707C50A22F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1F638D-BA3D-874D-B915-D398DB7F5D5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4160" yWindow="720" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1384,7 +1384,7 @@
       <pane xSplit="6" ySplit="20" topLeftCell="G105" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="E117" sqref="E117"/>
+      <selection pane="bottomRight" activeCell="G117" sqref="G117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4070,12 +4070,24 @@
       <c r="I116" s="19"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A117" s="20"/>
-      <c r="B117" s="19"/>
-      <c r="C117" s="19"/>
-      <c r="D117" s="23"/>
-      <c r="E117" s="23"/>
-      <c r="F117" s="23"/>
+      <c r="A117" s="20">
+        <v>44025</v>
+      </c>
+      <c r="B117" s="19">
+        <v>76</v>
+      </c>
+      <c r="C117" s="19">
+        <v>13</v>
+      </c>
+      <c r="D117" s="23">
+        <v>19</v>
+      </c>
+      <c r="E117" s="23">
+        <v>0</v>
+      </c>
+      <c r="F117" s="23">
+        <v>50</v>
+      </c>
       <c r="G117" s="23"/>
       <c r="H117" s="19"/>
       <c r="I117" s="19"/>

</xml_diff>

<commit_message>
Data through 2020-07-22 (some counties not updated due to HHS)
no update to counties with < 97% beds reporting due to HHS change
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C42C5A-0CC6-6948-9191-3D4141A6E94D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0A122F-2A33-5744-9AC8-B9D895C95C8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4160" yWindow="700" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -346,7 +346,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -374,6 +374,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -456,7 +462,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -569,6 +575,10 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1404,7 +1414,7 @@
       <pane xSplit="6" ySplit="20" topLeftCell="G105" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomRight" activeCell="A125" sqref="A125:A126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4297,12 +4307,24 @@
       <c r="I125" s="19"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A126" s="20"/>
-      <c r="B126" s="19"/>
-      <c r="C126" s="19"/>
-      <c r="D126" s="23"/>
-      <c r="E126" s="23"/>
-      <c r="F126" s="23"/>
+      <c r="A126" s="20">
+        <v>44034</v>
+      </c>
+      <c r="B126" s="19">
+        <v>97</v>
+      </c>
+      <c r="C126" s="48">
+        <v>23</v>
+      </c>
+      <c r="D126" s="23">
+        <v>27</v>
+      </c>
+      <c r="E126" s="47">
+        <v>3</v>
+      </c>
+      <c r="F126" s="47">
+        <v>55</v>
+      </c>
       <c r="G126" s="23"/>
       <c r="H126" s="19"/>
       <c r="I126" s="19"/>

</xml_diff>

<commit_message>
update SF only (others delayed due to HHS change)
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2503CFB0-AE10-074C-B68A-A0CE5B5E5057}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824C3339-7429-7240-AAC4-EC8C211BE60E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4160" yWindow="700" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1066,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:F12"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1313,6 +1313,26 @@
         <v>2</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>44025</v>
+      </c>
+      <c r="B13" s="3">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E13" s="3">
+        <v>7</v>
+      </c>
+      <c r="F13" s="3">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
@@ -1320,7 +1340,7 @@
     <mergeCell ref="E1:F1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A12" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A13" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>43831</formula1>
       <formula2>44196</formula2>
     </dataValidation>
@@ -1411,7 +1431,7 @@
   <dimension ref="A1:I305"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="20" topLeftCell="G107" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="20" topLeftCell="G116" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
       <selection pane="bottomRight" activeCell="B133" sqref="B133"/>
@@ -4368,7 +4388,7 @@
       <c r="E128" s="38">
         <v>1</v>
       </c>
-      <c r="F128" s="38">
+      <c r="F128" s="23">
         <v>56</v>
       </c>
       <c r="G128" s="23"/>
@@ -4391,7 +4411,7 @@
       <c r="E129" s="38">
         <v>1</v>
       </c>
-      <c r="F129" s="38">
+      <c r="F129" s="23">
         <v>56</v>
       </c>
       <c r="G129" s="23"/>
@@ -4399,12 +4419,24 @@
       <c r="I129" s="19"/>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A130" s="20"/>
-      <c r="B130" s="19"/>
-      <c r="C130" s="19"/>
-      <c r="D130" s="23"/>
-      <c r="E130" s="23"/>
-      <c r="F130" s="23"/>
+      <c r="A130" s="20">
+        <v>44038</v>
+      </c>
+      <c r="B130" s="19">
+        <v>105</v>
+      </c>
+      <c r="C130" s="39">
+        <v>27</v>
+      </c>
+      <c r="D130" s="23">
+        <v>34</v>
+      </c>
+      <c r="E130" s="38">
+        <v>1</v>
+      </c>
+      <c r="F130" s="38">
+        <v>56</v>
+      </c>
       <c r="G130" s="23"/>
       <c r="H130" s="19"/>
       <c r="I130" s="19"/>

</xml_diff>

<commit_message>
update Stanislaus, Tulare, Ventura
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9212C4F8-527B-3E45-90D1-18B6E06A9796}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3D2BC9-8AAF-314A-AE10-C44B5DB22624}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4160" yWindow="700" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9940" yWindow="1200" windowWidth="29440" windowHeight="19500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters with Distributions" sheetId="1" r:id="rId1"/>
@@ -545,6 +545,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -576,7 +577,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1065,8 +1065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1077,18 +1077,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38" t="s">
+      <c r="B1" s="39"/>
+      <c r="C1" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38" t="s">
+      <c r="D1" s="39"/>
+      <c r="E1" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="38"/>
+      <c r="F1" s="39"/>
     </row>
     <row r="2" spans="1:6" s="28" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
@@ -1447,11 +1447,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I305"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="20" topLeftCell="G117" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="20" topLeftCell="G119" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomRight" activeCell="B141" sqref="B141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1467,40 +1467,40 @@
   <sheetData>
     <row r="1" spans="1:9" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="16"/>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="43" t="s">
+      <c r="C1" s="43"/>
+      <c r="D1" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43" t="s">
+      <c r="E1" s="44"/>
+      <c r="F1" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="43"/>
-      <c r="H1" s="39" t="s">
+      <c r="G1" s="44"/>
+      <c r="H1" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="39"/>
+      <c r="I1" s="40"/>
     </row>
     <row r="2" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41" t="s">
+      <c r="C2" s="42"/>
+      <c r="D2" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="44" t="s">
+      <c r="E2" s="42"/>
+      <c r="F2" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="44"/>
-      <c r="H2" s="40" t="s">
+      <c r="G2" s="45"/>
+      <c r="H2" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="40"/>
+      <c r="I2" s="41"/>
     </row>
     <row r="3" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
@@ -4222,7 +4222,7 @@
         <v>1</v>
       </c>
       <c r="F120" s="23">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G120" s="23"/>
       <c r="H120" s="19"/>
@@ -4245,7 +4245,7 @@
         <v>2</v>
       </c>
       <c r="F121" s="23">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G121" s="23"/>
       <c r="H121" s="19"/>
@@ -4268,7 +4268,7 @@
         <v>1</v>
       </c>
       <c r="F122" s="23">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G122" s="23"/>
       <c r="H122" s="19"/>
@@ -4291,7 +4291,7 @@
         <v>2</v>
       </c>
       <c r="F123" s="23">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G123" s="23"/>
       <c r="H123" s="19"/>
@@ -4314,7 +4314,7 @@
         <v>1</v>
       </c>
       <c r="F124" s="23">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G124" s="23"/>
       <c r="H124" s="19"/>
@@ -4337,7 +4337,7 @@
         <v>3</v>
       </c>
       <c r="F125" s="23">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G125" s="23"/>
       <c r="H125" s="19"/>
@@ -4360,7 +4360,7 @@
         <v>1</v>
       </c>
       <c r="F126" s="23">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G126" s="23"/>
       <c r="H126" s="19"/>
@@ -4383,7 +4383,7 @@
         <v>3</v>
       </c>
       <c r="F127" s="23">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G127" s="23"/>
       <c r="H127" s="19"/>
@@ -4406,7 +4406,7 @@
         <v>6</v>
       </c>
       <c r="F128" s="23">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G128" s="23"/>
       <c r="H128" s="19"/>
@@ -4429,7 +4429,7 @@
         <v>5</v>
       </c>
       <c r="F129" s="23">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G129" s="23"/>
       <c r="H129" s="19"/>
@@ -4452,7 +4452,7 @@
         <v>1</v>
       </c>
       <c r="F130" s="23">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G130" s="23"/>
       <c r="H130" s="19"/>
@@ -4475,7 +4475,7 @@
         <v>2</v>
       </c>
       <c r="F131" s="23">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G131" s="23"/>
       <c r="H131" s="19"/>
@@ -4498,7 +4498,7 @@
         <v>2</v>
       </c>
       <c r="F132" s="23">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G132" s="23"/>
       <c r="H132" s="19"/>
@@ -4521,7 +4521,7 @@
         <v>3</v>
       </c>
       <c r="F133" s="23">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G133" s="23"/>
       <c r="H133" s="19"/>
@@ -4544,7 +4544,7 @@
         <v>1</v>
       </c>
       <c r="F134" s="23">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G134" s="23"/>
       <c r="H134" s="19"/>
@@ -4567,7 +4567,7 @@
         <v>1</v>
       </c>
       <c r="F135" s="23">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G135" s="23"/>
       <c r="H135" s="19"/>
@@ -4590,7 +4590,7 @@
         <v>4</v>
       </c>
       <c r="F136" s="23">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="G136" s="23"/>
       <c r="H136" s="19"/>
@@ -4612,8 +4612,8 @@
       <c r="E137" s="23">
         <v>1</v>
       </c>
-      <c r="F137" s="47">
-        <v>63</v>
+      <c r="F137" s="37">
+        <v>66</v>
       </c>
       <c r="G137" s="23"/>
       <c r="H137" s="19"/>
@@ -4635,8 +4635,8 @@
       <c r="E138" s="23">
         <v>1</v>
       </c>
-      <c r="F138" s="47">
-        <v>63</v>
+      <c r="F138" s="37">
+        <v>67</v>
       </c>
       <c r="G138" s="23"/>
       <c r="H138" s="19"/>
@@ -4659,8 +4659,8 @@
       <c r="E139" s="23">
         <v>0</v>
       </c>
-      <c r="F139" s="47">
-        <v>63</v>
+      <c r="F139" s="37">
+        <v>67</v>
       </c>
       <c r="G139" s="23"/>
       <c r="H139" s="19"/>
@@ -4683,20 +4683,32 @@
       <c r="E140" s="23">
         <v>1</v>
       </c>
-      <c r="F140" s="47">
-        <v>63</v>
+      <c r="F140" s="37">
+        <v>67</v>
       </c>
       <c r="G140" s="23"/>
       <c r="H140" s="19"/>
       <c r="I140" s="19"/>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A141" s="20"/>
-      <c r="B141" s="19"/>
-      <c r="C141" s="19"/>
-      <c r="D141" s="23"/>
-      <c r="E141" s="23"/>
-      <c r="F141" s="23"/>
+      <c r="A141" s="20">
+        <v>44049</v>
+      </c>
+      <c r="B141" s="19">
+        <v>80</v>
+      </c>
+      <c r="C141" s="19">
+        <v>11</v>
+      </c>
+      <c r="D141" s="23">
+        <v>29</v>
+      </c>
+      <c r="E141" s="23">
+        <v>0</v>
+      </c>
+      <c r="F141" s="38">
+        <v>67</v>
+      </c>
       <c r="G141" s="23"/>
       <c r="H141" s="19"/>
       <c r="I141" s="19"/>
@@ -6507,10 +6519,10 @@
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="46"/>
+      <c r="D4" s="47"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="30" t="s">

</xml_diff>

<commit_message>
Data through 2020-11-01 partial
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B3794D-0FC7-1D43-AE48-C5C95AF4B7D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B0AD7E-A4AB-964C-A185-C52A542252AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4160" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1545,10 +1545,10 @@
   <dimension ref="A1:I305"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="20" topLeftCell="G205" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="20" topLeftCell="G210" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="B223" sqref="B223"/>
+      <selection pane="bottomRight" activeCell="F230" sqref="F230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6789,23 +6789,47 @@
       <c r="I227" s="19"/>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A228" s="20"/>
-      <c r="B228" s="19"/>
-      <c r="C228" s="19"/>
-      <c r="D228" s="23"/>
-      <c r="E228" s="23"/>
-      <c r="F228" s="23"/>
+      <c r="A228" s="20">
+        <v>44136</v>
+      </c>
+      <c r="B228" s="19">
+        <v>35</v>
+      </c>
+      <c r="C228" s="19">
+        <v>2</v>
+      </c>
+      <c r="D228" s="23">
+        <v>11</v>
+      </c>
+      <c r="E228" s="23">
+        <v>1</v>
+      </c>
+      <c r="F228" s="23">
+        <v>148</v>
+      </c>
       <c r="G228" s="23"/>
       <c r="H228" s="19"/>
       <c r="I228" s="19"/>
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A229" s="20"/>
-      <c r="B229" s="19"/>
-      <c r="C229" s="19"/>
-      <c r="D229" s="23"/>
-      <c r="E229" s="23"/>
-      <c r="F229" s="23"/>
+      <c r="A229" s="20">
+        <v>44137</v>
+      </c>
+      <c r="B229" s="19">
+        <v>33</v>
+      </c>
+      <c r="C229" s="19">
+        <v>5</v>
+      </c>
+      <c r="D229" s="23">
+        <v>11</v>
+      </c>
+      <c r="E229" s="23">
+        <v>1</v>
+      </c>
+      <c r="F229" s="23">
+        <v>148</v>
+      </c>
       <c r="G229" s="23"/>
       <c r="H229" s="19"/>
       <c r="I229" s="19"/>

</xml_diff>

<commit_message>
Data through 2020-11-15 partial local
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE61DD3-BB83-D242-B7A7-36AC6419E1D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B55A9A0-E5D7-4145-9B58-B7F367FAD442}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4160" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1568,7 +1568,7 @@
       <pane xSplit="6" ySplit="20" topLeftCell="G219" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="G242" sqref="G242"/>
+      <selection pane="bottomRight" activeCell="G243" sqref="G243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7154,12 +7154,24 @@
       <c r="I242" s="19"/>
     </row>
     <row r="243" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A243" s="20"/>
-      <c r="B243" s="19"/>
-      <c r="C243" s="19"/>
-      <c r="D243" s="23"/>
-      <c r="E243" s="23"/>
-      <c r="F243" s="23"/>
+      <c r="A243" s="20">
+        <v>44151</v>
+      </c>
+      <c r="B243" s="19">
+        <v>39</v>
+      </c>
+      <c r="C243" s="19">
+        <v>11</v>
+      </c>
+      <c r="D243" s="23">
+        <v>11</v>
+      </c>
+      <c r="E243" s="23">
+        <v>3</v>
+      </c>
+      <c r="F243" s="23">
+        <v>156</v>
+      </c>
       <c r="G243" s="23"/>
       <c r="H243" s="19"/>
       <c r="I243" s="19"/>

</xml_diff>

<commit_message>
Data through 2020-11-23 (partial - continued from previous)
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DC758C-102D-DD41-A28E-80F9CB1B11F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A53A59-3AB3-8B40-A509-E656B674DA72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4160" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1268,7 +1268,7 @@
       <pane xSplit="6" ySplit="20" topLeftCell="G228" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="G248" sqref="G248"/>
+      <selection pane="bottomRight" activeCell="G249" sqref="G249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6992,12 +6992,24 @@
       <c r="I248" s="19"/>
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A249" s="20"/>
-      <c r="B249" s="19"/>
-      <c r="C249" s="19"/>
-      <c r="D249" s="23"/>
-      <c r="E249" s="23"/>
-      <c r="F249" s="23"/>
+      <c r="A249" s="20">
+        <v>44157</v>
+      </c>
+      <c r="B249" s="19">
+        <v>54</v>
+      </c>
+      <c r="C249" s="19">
+        <v>2</v>
+      </c>
+      <c r="D249" s="23">
+        <v>15</v>
+      </c>
+      <c r="E249" s="23">
+        <v>0</v>
+      </c>
+      <c r="F249" s="23">
+        <v>158</v>
+      </c>
       <c r="G249" s="23"/>
       <c r="H249" s="19"/>
       <c r="I249" s="19"/>

</xml_diff>

<commit_message>
SF data through 2020-12-07
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44519206-50EC-024A-AB87-77143542895B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A1E939-ACA4-E84B-96C5-6AEE7786468B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4160" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1268,7 +1268,7 @@
       <pane xSplit="6" ySplit="20" topLeftCell="G241" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="G263" sqref="G263"/>
+      <selection pane="bottomRight" activeCell="F265" sqref="F265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7337,12 +7337,24 @@
       <c r="I263" s="19"/>
     </row>
     <row r="264" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A264" s="20"/>
-      <c r="B264" s="19"/>
-      <c r="C264" s="19"/>
-      <c r="D264" s="23"/>
-      <c r="E264" s="23"/>
-      <c r="F264" s="23"/>
+      <c r="A264" s="20">
+        <v>44172</v>
+      </c>
+      <c r="B264" s="19">
+        <v>119</v>
+      </c>
+      <c r="C264" s="19">
+        <v>6</v>
+      </c>
+      <c r="D264" s="23">
+        <v>30</v>
+      </c>
+      <c r="E264" s="23">
+        <v>0</v>
+      </c>
+      <c r="F264" s="23">
+        <v>164</v>
+      </c>
       <c r="G264" s="23"/>
       <c r="H264" s="19"/>
       <c r="I264" s="19"/>

</xml_diff>

<commit_message>
SF data through 2020-12-08
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A1E939-ACA4-E84B-96C5-6AEE7786468B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6888E36E-3B2D-364B-A420-6049DFE1A72B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4160" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1268,7 +1268,7 @@
       <pane xSplit="6" ySplit="20" topLeftCell="G241" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="F265" sqref="F265"/>
+      <selection pane="bottomRight" activeCell="B261" sqref="B261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7360,12 +7360,24 @@
       <c r="I264" s="19"/>
     </row>
     <row r="265" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A265" s="20"/>
-      <c r="B265" s="19"/>
-      <c r="C265" s="19"/>
-      <c r="D265" s="23"/>
-      <c r="E265" s="23"/>
-      <c r="F265" s="23"/>
+      <c r="A265" s="20">
+        <v>44173</v>
+      </c>
+      <c r="B265" s="19">
+        <v>125</v>
+      </c>
+      <c r="C265" s="19">
+        <v>7</v>
+      </c>
+      <c r="D265" s="23">
+        <v>32</v>
+      </c>
+      <c r="E265" s="23">
+        <v>1</v>
+      </c>
+      <c r="F265" s="23">
+        <v>164</v>
+      </c>
       <c r="G265" s="23"/>
       <c r="H265" s="19"/>
       <c r="I265" s="19"/>

</xml_diff>

<commit_message>
SF data through 2020-12-09
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6888E36E-3B2D-364B-A420-6049DFE1A72B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D72E095-D275-8148-BC8E-C08D4D773399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4160" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1265,10 +1265,10 @@
   <dimension ref="A1:I305"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="20" topLeftCell="G241" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="20" topLeftCell="G254" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="B261" sqref="B261"/>
+      <selection pane="bottomRight" activeCell="F267" sqref="F267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7383,12 +7383,24 @@
       <c r="I265" s="19"/>
     </row>
     <row r="266" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A266" s="20"/>
-      <c r="B266" s="19"/>
-      <c r="C266" s="19"/>
-      <c r="D266" s="23"/>
-      <c r="E266" s="23"/>
-      <c r="F266" s="23"/>
+      <c r="A266" s="20">
+        <v>44174</v>
+      </c>
+      <c r="B266" s="19">
+        <v>124</v>
+      </c>
+      <c r="C266" s="19">
+        <v>4</v>
+      </c>
+      <c r="D266" s="23">
+        <v>33</v>
+      </c>
+      <c r="E266" s="23">
+        <v>1</v>
+      </c>
+      <c r="F266" s="23">
+        <v>164</v>
+      </c>
       <c r="G266" s="23"/>
       <c r="H266" s="19"/>
       <c r="I266" s="19"/>

</xml_diff>

<commit_message>
SF data through 2020-12-10
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D72E095-D275-8148-BC8E-C08D4D773399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0ED277-3F20-F643-9DA2-EFF318FA0C4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4160" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1268,7 +1268,7 @@
       <pane xSplit="6" ySplit="20" topLeftCell="G254" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="F267" sqref="F267"/>
+      <selection pane="bottomRight" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7406,12 +7406,24 @@
       <c r="I266" s="19"/>
     </row>
     <row r="267" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A267" s="20"/>
-      <c r="B267" s="19"/>
-      <c r="C267" s="19"/>
-      <c r="D267" s="23"/>
-      <c r="E267" s="23"/>
-      <c r="F267" s="23"/>
+      <c r="A267" s="20">
+        <v>44175</v>
+      </c>
+      <c r="B267" s="19">
+        <v>134</v>
+      </c>
+      <c r="C267" s="19">
+        <v>8</v>
+      </c>
+      <c r="D267" s="23">
+        <v>33</v>
+      </c>
+      <c r="E267" s="23">
+        <v>0</v>
+      </c>
+      <c r="F267" s="23">
+        <v>165</v>
+      </c>
       <c r="G267" s="23"/>
       <c r="H267" s="19"/>
       <c r="I267" s="19"/>

</xml_diff>

<commit_message>
SF data through 2020-12-12
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D238C6A-97BA-FD4B-9161-B1FD748BEB20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8993E3D6-4964-E348-A0D2-26CE34BB7B46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4160" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters with Distributions" sheetId="1" r:id="rId1"/>
@@ -1264,11 +1264,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I305"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="6" ySplit="20" topLeftCell="G246" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="B266" sqref="B266"/>
+      <selection pane="bottomRight" activeCell="G269" sqref="G269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7452,12 +7452,24 @@
       <c r="I268" s="19"/>
     </row>
     <row r="269" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A269" s="20"/>
-      <c r="B269" s="19"/>
-      <c r="C269" s="19"/>
-      <c r="D269" s="23"/>
-      <c r="E269" s="23"/>
-      <c r="F269" s="23"/>
+      <c r="A269" s="20">
+        <v>44177</v>
+      </c>
+      <c r="B269" s="19">
+        <v>146</v>
+      </c>
+      <c r="C269" s="19">
+        <v>8</v>
+      </c>
+      <c r="D269" s="23">
+        <v>37</v>
+      </c>
+      <c r="E269" s="23">
+        <v>1</v>
+      </c>
+      <c r="F269" s="23">
+        <v>167</v>
+      </c>
       <c r="G269" s="23"/>
       <c r="H269" s="19"/>
       <c r="I269" s="19"/>
@@ -7957,8 +7969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8065,7 +8077,7 @@
         <v>37</v>
       </c>
       <c r="B8" s="3">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="C8">
         <v>1000</v>

</xml_diff>

<commit_message>
SF data through 2020-12-13
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8993E3D6-4964-E348-A0D2-26CE34BB7B46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D856E01F-6166-8340-8DC1-1A578393C5EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters with Distributions" sheetId="1" r:id="rId1"/>
@@ -1264,11 +1264,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I305"/>
   <sheetViews>
-    <sheetView zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="20" topLeftCell="G246" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="20" topLeftCell="G252" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="G269" sqref="G269"/>
+      <selection pane="bottomRight" activeCell="G270" sqref="G270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7475,12 +7475,24 @@
       <c r="I269" s="19"/>
     </row>
     <row r="270" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A270" s="20"/>
-      <c r="B270" s="19"/>
-      <c r="C270" s="19"/>
-      <c r="D270" s="23"/>
-      <c r="E270" s="23"/>
-      <c r="F270" s="23"/>
+      <c r="A270" s="20">
+        <v>44178</v>
+      </c>
+      <c r="B270" s="19">
+        <v>158</v>
+      </c>
+      <c r="C270" s="19">
+        <v>8</v>
+      </c>
+      <c r="D270" s="23">
+        <v>40</v>
+      </c>
+      <c r="E270" s="23">
+        <v>1</v>
+      </c>
+      <c r="F270" s="23">
+        <v>167</v>
+      </c>
       <c r="G270" s="23"/>
       <c r="H270" s="19"/>
       <c r="I270" s="19"/>
@@ -7969,7 +7981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
SF data through 2020-12-14
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D856E01F-6166-8340-8DC1-1A578393C5EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B41A78-CCE0-E743-B012-5904EA315FFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1268,7 +1268,7 @@
       <pane xSplit="6" ySplit="20" topLeftCell="G252" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="G270" sqref="G270"/>
+      <selection pane="bottomRight" activeCell="F272" sqref="F272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7498,12 +7498,24 @@
       <c r="I270" s="19"/>
     </row>
     <row r="271" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A271" s="20"/>
-      <c r="B271" s="19"/>
-      <c r="C271" s="19"/>
-      <c r="D271" s="23"/>
-      <c r="E271" s="23"/>
-      <c r="F271" s="23"/>
+      <c r="A271" s="20">
+        <v>44179</v>
+      </c>
+      <c r="B271" s="19">
+        <v>149</v>
+      </c>
+      <c r="C271" s="19">
+        <v>8</v>
+      </c>
+      <c r="D271" s="23">
+        <v>42</v>
+      </c>
+      <c r="E271" s="23">
+        <v>0</v>
+      </c>
+      <c r="F271" s="23">
+        <v>167</v>
+      </c>
       <c r="G271" s="23"/>
       <c r="H271" s="19"/>
       <c r="I271" s="19"/>

</xml_diff>

<commit_message>
SF data through 2020-12-17
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C84286-AC22-DF44-9E94-215075187342}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1258320B-0661-C84B-B8FB-C056DBC37D64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters with Distributions" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="86">
   <si>
     <t>Number of Days from Infection to Becoming Infectious (Latent Period)</t>
   </si>
@@ -285,6 +285,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>warmup</t>
   </si>
 </sst>
 </file>
@@ -891,7 +894,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1268,7 +1271,7 @@
       <pane xSplit="6" ySplit="20" topLeftCell="G257" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="F274" sqref="F274"/>
+      <selection pane="bottomRight" activeCell="F275" sqref="F275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6781,12 +6784,24 @@
       <c r="I273" s="19"/>
     </row>
     <row r="274" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A274" s="20"/>
-      <c r="B274" s="19"/>
-      <c r="C274" s="19"/>
-      <c r="D274" s="23"/>
-      <c r="E274" s="23"/>
-      <c r="F274" s="23"/>
+      <c r="A274" s="20">
+        <v>44182</v>
+      </c>
+      <c r="B274" s="19">
+        <v>161</v>
+      </c>
+      <c r="C274" s="19">
+        <v>9</v>
+      </c>
+      <c r="D274" s="23">
+        <v>41</v>
+      </c>
+      <c r="E274" s="23">
+        <v>2</v>
+      </c>
+      <c r="F274" s="23">
+        <v>172</v>
+      </c>
       <c r="G274" s="23"/>
       <c r="H274" s="19"/>
       <c r="I274" s="19"/>
@@ -7229,10 +7244,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7339,7 +7354,7 @@
         <v>37</v>
       </c>
       <c r="B8" s="3">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="C8">
         <v>1000</v>
@@ -7349,64 +7364,73 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" t="s">
-        <v>54</v>
-      </c>
+      <c r="A9" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C9"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="3">
-        <v>25</v>
-      </c>
-      <c r="C10">
-        <v>250</v>
+        <v>38</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="3">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C11">
-        <v>10</v>
-      </c>
-      <c r="D11">
-        <v>13</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="3">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B13" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="C13">
         <v>0.8</v>
       </c>
-      <c r="C12">
-        <v>0.8</v>
-      </c>
-      <c r="D12">
+      <c r="D13">
         <v>0.9</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="34">
+      <c r="B14" s="34">
         <v>0.3</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C14" s="1">
         <v>0.3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
SF data through 2020-12-18
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1258320B-0661-C84B-B8FB-C056DBC37D64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABBC0B2-85DA-1441-BE9A-69A418722CA2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters with Distributions" sheetId="1" r:id="rId1"/>
@@ -1267,11 +1267,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I305"/>
   <sheetViews>
-    <sheetView zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="6" ySplit="20" topLeftCell="G257" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="F275" sqref="F275"/>
+      <selection pane="bottomRight" activeCell="F276" sqref="F276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6807,12 +6807,24 @@
       <c r="I274" s="19"/>
     </row>
     <row r="275" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A275" s="20"/>
-      <c r="B275" s="19"/>
-      <c r="C275" s="19"/>
-      <c r="D275" s="23"/>
-      <c r="E275" s="23"/>
-      <c r="F275" s="23"/>
+      <c r="A275" s="20">
+        <v>44183</v>
+      </c>
+      <c r="B275" s="19">
+        <v>175</v>
+      </c>
+      <c r="C275" s="19">
+        <v>6</v>
+      </c>
+      <c r="D275" s="23">
+        <v>40</v>
+      </c>
+      <c r="E275" s="23">
+        <v>0</v>
+      </c>
+      <c r="F275" s="23">
+        <v>173</v>
+      </c>
       <c r="G275" s="23"/>
       <c r="H275" s="19"/>
       <c r="I275" s="19"/>
@@ -7246,7 +7258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Santa Clara data through 2020-12-21
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB1C9BE-FF90-B541-9EED-86702BB96505}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEB78B2-D818-D245-9C31-16B545D3CE32}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters with Distributions" sheetId="1" r:id="rId1"/>
@@ -352,7 +352,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,12 +380,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -468,7 +462,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -552,10 +546,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1087,18 +1077,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="39"/>
+      <c r="C1" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41" t="s">
+      <c r="D1" s="39"/>
+      <c r="E1" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="41"/>
+      <c r="F1" s="39"/>
     </row>
     <row r="2" spans="1:6" s="28" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
@@ -1204,7 +1194,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1277,11 +1267,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I305"/>
   <sheetViews>
-    <sheetView zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="6" ySplit="20" topLeftCell="G257" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="C271" sqref="C271"/>
+      <selection pane="bottomRight" activeCell="G277" sqref="G277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1297,40 +1287,40 @@
   <sheetData>
     <row r="1" spans="1:9" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="16"/>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="46" t="s">
+      <c r="C1" s="43"/>
+      <c r="D1" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46" t="s">
+      <c r="E1" s="44"/>
+      <c r="F1" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="46"/>
-      <c r="H1" s="42" t="s">
+      <c r="G1" s="44"/>
+      <c r="H1" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="42"/>
+      <c r="I1" s="40"/>
     </row>
     <row r="2" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44" t="s">
+      <c r="C2" s="42"/>
+      <c r="D2" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="44"/>
-      <c r="F2" s="47" t="s">
+      <c r="E2" s="42"/>
+      <c r="F2" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="47"/>
-      <c r="H2" s="43" t="s">
+      <c r="G2" s="45"/>
+      <c r="H2" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="43"/>
+      <c r="I2" s="41"/>
     </row>
     <row r="3" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
@@ -6844,16 +6834,16 @@
         <v>44184</v>
       </c>
       <c r="B276" s="19">
-        <v>180</v>
-      </c>
-      <c r="C276" s="39">
-        <v>6</v>
+        <v>179</v>
+      </c>
+      <c r="C276" s="19">
+        <v>4</v>
       </c>
       <c r="D276" s="23">
         <v>43</v>
       </c>
-      <c r="E276" s="40">
-        <v>0</v>
+      <c r="E276" s="23">
+        <v>1</v>
       </c>
       <c r="F276" s="23">
         <v>176</v>
@@ -6863,12 +6853,24 @@
       <c r="I276" s="19"/>
     </row>
     <row r="277" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A277" s="20"/>
-      <c r="B277" s="19"/>
-      <c r="C277" s="19"/>
-      <c r="D277" s="23"/>
-      <c r="E277" s="23"/>
-      <c r="F277" s="23"/>
+      <c r="A277" s="20">
+        <v>44185</v>
+      </c>
+      <c r="B277" s="19">
+        <v>173</v>
+      </c>
+      <c r="C277" s="19">
+        <v>9</v>
+      </c>
+      <c r="D277" s="23">
+        <v>46</v>
+      </c>
+      <c r="E277" s="23">
+        <v>1</v>
+      </c>
+      <c r="F277" s="23">
+        <v>176</v>
+      </c>
       <c r="G277" s="23"/>
       <c r="H277" s="19"/>
       <c r="I277" s="19"/>
@@ -7144,7 +7146,7 @@
       <formula1>43831</formula1>
       <formula2>44561</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I299 H63:H299 H5:H60 F133:F148 B71:B323 C5:C322 B5:B64" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I299 H63:H299 H5:H60 F133:F148 B71:B323 B5:B64 C5:C322" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>0</formula1>
       <formula2>10000000</formula2>
     </dataValidation>
@@ -7183,10 +7185,10 @@
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="49"/>
+      <c r="D4" s="47"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="30" t="s">

</xml_diff>

<commit_message>
SF data through 2020-12-21
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEB78B2-D818-D245-9C31-16B545D3CE32}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E779D5DC-A271-9748-8ECA-0892582B9E4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1271,7 +1271,7 @@
       <pane xSplit="6" ySplit="20" topLeftCell="G257" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="G277" sqref="G277"/>
+      <selection pane="bottomRight" activeCell="G278" sqref="G278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6876,12 +6876,24 @@
       <c r="I277" s="19"/>
     </row>
     <row r="278" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A278" s="20"/>
-      <c r="B278" s="19"/>
-      <c r="C278" s="19"/>
-      <c r="D278" s="23"/>
-      <c r="E278" s="23"/>
-      <c r="F278" s="23"/>
+      <c r="A278" s="20">
+        <v>44186</v>
+      </c>
+      <c r="B278" s="19">
+        <v>167</v>
+      </c>
+      <c r="C278" s="19">
+        <v>10</v>
+      </c>
+      <c r="D278" s="23">
+        <v>49</v>
+      </c>
+      <c r="E278" s="23">
+        <v>0</v>
+      </c>
+      <c r="F278" s="23">
+        <v>176</v>
+      </c>
       <c r="G278" s="23"/>
       <c r="H278" s="19"/>
       <c r="I278" s="19"/>

</xml_diff>

<commit_message>
SF data through 2020-12-22
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E779D5DC-A271-9748-8ECA-0892582B9E4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07FBD0F3-98E1-8D45-83E3-DABA6F91609C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1271,7 +1271,7 @@
       <pane xSplit="6" ySplit="20" topLeftCell="G257" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="G278" sqref="G278"/>
+      <selection pane="bottomRight" activeCell="B277" sqref="B277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6899,12 +6899,24 @@
       <c r="I278" s="19"/>
     </row>
     <row r="279" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A279" s="20"/>
-      <c r="B279" s="19"/>
-      <c r="C279" s="19"/>
-      <c r="D279" s="23"/>
-      <c r="E279" s="23"/>
-      <c r="F279" s="23"/>
+      <c r="A279" s="20">
+        <v>44187</v>
+      </c>
+      <c r="B279" s="19">
+        <v>175</v>
+      </c>
+      <c r="C279" s="19">
+        <v>13</v>
+      </c>
+      <c r="D279" s="23">
+        <v>47</v>
+      </c>
+      <c r="E279" s="23">
+        <v>1</v>
+      </c>
+      <c r="F279" s="23">
+        <v>176</v>
+      </c>
       <c r="G279" s="23"/>
       <c r="H279" s="19"/>
       <c r="I279" s="19"/>

</xml_diff>

<commit_message>
SF data through 2020-12-23
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07FBD0F3-98E1-8D45-83E3-DABA6F91609C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B9F730-74EB-C24F-9990-ACD3746D1C14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1271,7 +1271,7 @@
       <pane xSplit="6" ySplit="20" topLeftCell="G257" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="B277" sqref="B277"/>
+      <selection pane="bottomRight" activeCell="F281" sqref="F281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6922,12 +6922,24 @@
       <c r="I279" s="19"/>
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A280" s="20"/>
-      <c r="B280" s="19"/>
-      <c r="C280" s="19"/>
-      <c r="D280" s="23"/>
-      <c r="E280" s="23"/>
-      <c r="F280" s="23"/>
+      <c r="A280" s="20">
+        <v>44188</v>
+      </c>
+      <c r="B280" s="19">
+        <v>182</v>
+      </c>
+      <c r="C280" s="19">
+        <v>12</v>
+      </c>
+      <c r="D280" s="23">
+        <v>54</v>
+      </c>
+      <c r="E280" s="23">
+        <v>0</v>
+      </c>
+      <c r="F280" s="23">
+        <v>178</v>
+      </c>
       <c r="G280" s="23"/>
       <c r="H280" s="19"/>
       <c r="I280" s="19"/>

</xml_diff>

<commit_message>
SF data through 2020-12-25
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B9F730-74EB-C24F-9990-ACD3746D1C14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6BEA52-C9D5-A24D-9C3C-6126C50BD101}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1271,7 +1271,7 @@
       <pane xSplit="6" ySplit="20" topLeftCell="G257" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="F281" sqref="F281"/>
+      <selection pane="bottomRight" activeCell="F283" sqref="F283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6945,23 +6945,47 @@
       <c r="I280" s="19"/>
     </row>
     <row r="281" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A281" s="20"/>
-      <c r="B281" s="19"/>
-      <c r="C281" s="19"/>
-      <c r="D281" s="23"/>
-      <c r="E281" s="23"/>
-      <c r="F281" s="23"/>
+      <c r="A281" s="20">
+        <v>44189</v>
+      </c>
+      <c r="B281" s="19">
+        <v>173</v>
+      </c>
+      <c r="C281" s="19">
+        <v>6</v>
+      </c>
+      <c r="D281" s="23">
+        <v>51</v>
+      </c>
+      <c r="E281" s="23">
+        <v>1</v>
+      </c>
+      <c r="F281" s="23">
+        <v>178</v>
+      </c>
       <c r="G281" s="23"/>
       <c r="H281" s="22"/>
       <c r="I281" s="22"/>
     </row>
     <row r="282" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A282" s="20"/>
-      <c r="B282" s="19"/>
-      <c r="C282" s="19"/>
-      <c r="D282" s="23"/>
-      <c r="E282" s="23"/>
-      <c r="F282" s="23"/>
+      <c r="A282" s="20">
+        <v>44190</v>
+      </c>
+      <c r="B282" s="19">
+        <v>185</v>
+      </c>
+      <c r="C282" s="19">
+        <v>4</v>
+      </c>
+      <c r="D282" s="23">
+        <v>49</v>
+      </c>
+      <c r="E282" s="23">
+        <v>1</v>
+      </c>
+      <c r="F282" s="23">
+        <v>181</v>
+      </c>
       <c r="G282" s="23"/>
     </row>
     <row r="283" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
SF data through 2020-12-26
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6BEA52-C9D5-A24D-9C3C-6126C50BD101}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8FE67C-D1E4-E647-A574-58991E7E9409}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1268,10 +1268,10 @@
   <dimension ref="A1:I305"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="20" topLeftCell="G257" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="20" topLeftCell="G272" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="F283" sqref="F283"/>
+      <selection pane="bottomRight" activeCell="F284" sqref="F284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6989,12 +6989,24 @@
       <c r="G282" s="23"/>
     </row>
     <row r="283" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A283" s="20"/>
-      <c r="B283" s="19"/>
-      <c r="C283" s="19"/>
-      <c r="D283" s="23"/>
-      <c r="E283" s="23"/>
-      <c r="F283" s="23"/>
+      <c r="A283" s="20">
+        <v>44191</v>
+      </c>
+      <c r="B283" s="19">
+        <v>188</v>
+      </c>
+      <c r="C283" s="19">
+        <v>5</v>
+      </c>
+      <c r="D283" s="23">
+        <v>48</v>
+      </c>
+      <c r="E283" s="23">
+        <v>0</v>
+      </c>
+      <c r="F283" s="23">
+        <v>181</v>
+      </c>
       <c r="G283" s="23"/>
     </row>
     <row r="284" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
SF data through 2020-12-27
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8FE67C-D1E4-E647-A574-58991E7E9409}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50E34B2-BF29-CC42-A152-CF651FB7937C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1271,7 +1271,7 @@
       <pane xSplit="6" ySplit="20" topLeftCell="G272" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="F284" sqref="F284"/>
+      <selection pane="bottomRight" activeCell="F285" sqref="F285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7010,12 +7010,24 @@
       <c r="G283" s="23"/>
     </row>
     <row r="284" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A284" s="20"/>
-      <c r="B284" s="19"/>
-      <c r="C284" s="19"/>
-      <c r="D284" s="23"/>
-      <c r="E284" s="23"/>
-      <c r="F284" s="23"/>
+      <c r="A284" s="20">
+        <v>44192</v>
+      </c>
+      <c r="B284" s="19">
+        <v>197</v>
+      </c>
+      <c r="C284" s="19">
+        <v>5</v>
+      </c>
+      <c r="D284" s="23">
+        <v>50</v>
+      </c>
+      <c r="E284" s="23">
+        <v>2</v>
+      </c>
+      <c r="F284" s="23">
+        <v>182</v>
+      </c>
       <c r="G284" s="23"/>
     </row>
     <row r="285" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
SF data through 2020-12-28
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50E34B2-BF29-CC42-A152-CF651FB7937C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752EABEC-26B9-B44D-B4CF-9BABF561E34A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1271,7 +1271,7 @@
       <pane xSplit="6" ySplit="20" topLeftCell="G272" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="F285" sqref="F285"/>
+      <selection pane="bottomRight" activeCell="F286" sqref="F286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7031,12 +7031,24 @@
       <c r="G284" s="23"/>
     </row>
     <row r="285" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A285" s="20"/>
-      <c r="B285" s="19"/>
-      <c r="C285" s="19"/>
-      <c r="D285" s="23"/>
-      <c r="E285" s="23"/>
-      <c r="F285" s="23"/>
+      <c r="A285" s="20">
+        <v>44193</v>
+      </c>
+      <c r="B285" s="19">
+        <v>215</v>
+      </c>
+      <c r="C285" s="19">
+        <v>6</v>
+      </c>
+      <c r="D285" s="23">
+        <v>54</v>
+      </c>
+      <c r="E285" s="23">
+        <v>3</v>
+      </c>
+      <c r="F285" s="23">
+        <v>182</v>
+      </c>
       <c r="G285" s="23"/>
     </row>
     <row r="286" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
SF data through 2020-12-29
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752EABEC-26B9-B44D-B4CF-9BABF561E34A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907F9267-5504-0B4D-B72D-31C341815D56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1271,7 +1271,7 @@
       <pane xSplit="6" ySplit="20" topLeftCell="G272" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="F286" sqref="F286"/>
+      <selection pane="bottomRight" activeCell="F287" sqref="F287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7052,12 +7052,24 @@
       <c r="G285" s="23"/>
     </row>
     <row r="286" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A286" s="20"/>
-      <c r="B286" s="19"/>
-      <c r="C286" s="19"/>
-      <c r="D286" s="23"/>
-      <c r="E286" s="23"/>
-      <c r="F286" s="23"/>
+      <c r="A286" s="20">
+        <v>44194</v>
+      </c>
+      <c r="B286" s="19">
+        <v>221</v>
+      </c>
+      <c r="C286" s="19">
+        <v>3</v>
+      </c>
+      <c r="D286" s="23">
+        <v>57</v>
+      </c>
+      <c r="E286" s="23">
+        <v>2</v>
+      </c>
+      <c r="F286" s="23">
+        <v>182</v>
+      </c>
       <c r="G286" s="23"/>
     </row>
     <row r="287" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
SF data through 2020-12-31
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD728AB-AA7B-D348-9E59-1836F81683B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF181F4-D297-B746-8A15-E4F4B84B01A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1271,7 +1271,7 @@
       <pane xSplit="6" ySplit="20" topLeftCell="G272" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="F288" sqref="F288"/>
+      <selection pane="bottomRight" activeCell="F289" sqref="F289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7077,7 +7077,7 @@
         <v>44195</v>
       </c>
       <c r="B287" s="19">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C287" s="19">
         <v>8</v>
@@ -7094,12 +7094,24 @@
       <c r="G287" s="23"/>
     </row>
     <row r="288" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A288" s="20"/>
-      <c r="B288" s="19"/>
-      <c r="C288" s="19"/>
-      <c r="D288" s="23"/>
-      <c r="E288" s="23"/>
-      <c r="F288" s="23"/>
+      <c r="A288" s="20">
+        <v>44196</v>
+      </c>
+      <c r="B288" s="19">
+        <v>216</v>
+      </c>
+      <c r="C288" s="19">
+        <v>5</v>
+      </c>
+      <c r="D288" s="23">
+        <v>54</v>
+      </c>
+      <c r="E288" s="23">
+        <v>1</v>
+      </c>
+      <c r="F288" s="23">
+        <v>186</v>
+      </c>
       <c r="G288" s="23"/>
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
SF data through 2021-01-01
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF181F4-D297-B746-8A15-E4F4B84B01A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E73BAE9-51CB-5849-A697-3A30226B320C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1271,7 +1271,7 @@
       <pane xSplit="6" ySplit="20" topLeftCell="G272" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="F289" sqref="F289"/>
+      <selection pane="bottomRight" activeCell="F290" sqref="F290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7115,12 +7115,24 @@
       <c r="G288" s="23"/>
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A289" s="20"/>
-      <c r="B289" s="19"/>
-      <c r="C289" s="19"/>
-      <c r="D289" s="23"/>
-      <c r="E289" s="23"/>
-      <c r="F289" s="23"/>
+      <c r="A289" s="20">
+        <v>44197</v>
+      </c>
+      <c r="B289" s="19">
+        <v>219</v>
+      </c>
+      <c r="C289" s="19">
+        <v>5</v>
+      </c>
+      <c r="D289" s="23">
+        <v>56</v>
+      </c>
+      <c r="E289" s="23">
+        <v>1</v>
+      </c>
+      <c r="F289" s="23">
+        <v>189</v>
+      </c>
       <c r="G289" s="23"/>
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
SF data through 2021-01-02
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E73BAE9-51CB-5849-A697-3A30226B320C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421C17B7-7366-294A-B932-4FFC01C15FD5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1271,7 +1271,7 @@
       <pane xSplit="6" ySplit="20" topLeftCell="G272" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="F290" sqref="F290"/>
+      <selection pane="bottomRight" activeCell="B290" sqref="B290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7136,12 +7136,24 @@
       <c r="G289" s="23"/>
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A290" s="20"/>
-      <c r="B290" s="19"/>
-      <c r="C290" s="19"/>
-      <c r="D290" s="23"/>
-      <c r="E290" s="23"/>
-      <c r="F290" s="23"/>
+      <c r="A290" s="20">
+        <v>44198</v>
+      </c>
+      <c r="B290" s="19">
+        <v>211</v>
+      </c>
+      <c r="C290" s="19">
+        <v>5</v>
+      </c>
+      <c r="D290" s="23">
+        <v>54</v>
+      </c>
+      <c r="E290" s="23">
+        <v>1</v>
+      </c>
+      <c r="F290" s="23">
+        <v>194</v>
+      </c>
       <c r="G290" s="23"/>
     </row>
     <row r="291" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
BayArea data through 2021-01-03
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421C17B7-7366-294A-B932-4FFC01C15FD5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789064EC-F962-BF41-810A-BDF2618B6916}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1271,7 +1271,7 @@
       <pane xSplit="6" ySplit="20" topLeftCell="G272" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="B290" sqref="B290"/>
+      <selection pane="bottomRight" activeCell="F292" sqref="F292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7056,13 +7056,13 @@
         <v>44194</v>
       </c>
       <c r="B286" s="19">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C286" s="19">
         <v>3</v>
       </c>
       <c r="D286" s="23">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E286" s="23">
         <v>2</v>
@@ -7077,7 +7077,7 @@
         <v>44195</v>
       </c>
       <c r="B287" s="19">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C287" s="19">
         <v>8</v>
@@ -7098,13 +7098,13 @@
         <v>44196</v>
       </c>
       <c r="B288" s="19">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C288" s="19">
         <v>5</v>
       </c>
       <c r="D288" s="23">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E288" s="23">
         <v>1</v>
@@ -7119,13 +7119,13 @@
         <v>44197</v>
       </c>
       <c r="B289" s="19">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C289" s="19">
         <v>5</v>
       </c>
       <c r="D289" s="23">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E289" s="23">
         <v>1</v>
@@ -7140,13 +7140,13 @@
         <v>44198</v>
       </c>
       <c r="B290" s="19">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C290" s="19">
         <v>5</v>
       </c>
       <c r="D290" s="23">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E290" s="23">
         <v>1</v>
@@ -7157,12 +7157,24 @@
       <c r="G290" s="23"/>
     </row>
     <row r="291" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A291" s="20"/>
-      <c r="B291" s="19"/>
-      <c r="C291" s="19"/>
-      <c r="D291" s="23"/>
-      <c r="E291" s="23"/>
-      <c r="F291" s="23"/>
+      <c r="A291" s="20">
+        <v>44199</v>
+      </c>
+      <c r="B291" s="19">
+        <v>214</v>
+      </c>
+      <c r="C291" s="19">
+        <v>5</v>
+      </c>
+      <c r="D291" s="23">
+        <v>53</v>
+      </c>
+      <c r="E291" s="23">
+        <v>2</v>
+      </c>
+      <c r="F291" s="23">
+        <v>194</v>
+      </c>
       <c r="G291" s="23"/>
     </row>
     <row r="292" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
SF data through 2021-01-04
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789064EC-F962-BF41-810A-BDF2618B6916}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398B387F-C340-174A-A322-A0127C69DD19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1271,7 +1271,7 @@
       <pane xSplit="6" ySplit="20" topLeftCell="G272" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="F292" sqref="F292"/>
+      <selection pane="bottomRight" activeCell="F293" sqref="F293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7178,12 +7178,24 @@
       <c r="G291" s="23"/>
     </row>
     <row r="292" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A292" s="20"/>
-      <c r="B292" s="19"/>
-      <c r="C292" s="19"/>
-      <c r="D292" s="23"/>
-      <c r="E292" s="23"/>
-      <c r="F292" s="23"/>
+      <c r="A292" s="20">
+        <v>44200</v>
+      </c>
+      <c r="B292" s="19">
+        <v>222</v>
+      </c>
+      <c r="C292" s="19">
+        <v>8</v>
+      </c>
+      <c r="D292" s="23">
+        <v>60</v>
+      </c>
+      <c r="E292" s="23">
+        <v>1</v>
+      </c>
+      <c r="F292" s="23">
+        <v>194</v>
+      </c>
       <c r="G292" s="23"/>
     </row>
     <row r="293" spans="1:7" x14ac:dyDescent="0.2">
@@ -7451,7 +7463,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7604,7 +7616,7 @@
         <v>40</v>
       </c>
       <c r="B12" s="3">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C12">
         <v>10</v>

</xml_diff>

<commit_message>
SF data through 2021-01-05
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398B387F-C340-174A-A322-A0127C69DD19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DB7B84-5C99-BB41-9F4A-F3DF600F7B2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1271,7 +1271,7 @@
       <pane xSplit="6" ySplit="20" topLeftCell="G272" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="F293" sqref="F293"/>
+      <selection pane="bottomRight" activeCell="F294" sqref="F294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7199,12 +7199,24 @@
       <c r="G292" s="23"/>
     </row>
     <row r="293" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A293" s="20"/>
-      <c r="B293" s="19"/>
-      <c r="C293" s="19"/>
-      <c r="D293" s="23"/>
-      <c r="E293" s="23"/>
-      <c r="F293" s="23"/>
+      <c r="A293" s="20">
+        <v>44201</v>
+      </c>
+      <c r="B293" s="19">
+        <v>235</v>
+      </c>
+      <c r="C293" s="19">
+        <v>10</v>
+      </c>
+      <c r="D293" s="23">
+        <v>59</v>
+      </c>
+      <c r="E293" s="23">
+        <v>1</v>
+      </c>
+      <c r="F293" s="23">
+        <v>198</v>
+      </c>
       <c r="G293" s="23"/>
     </row>
     <row r="294" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Santa Clara data through 2021-01-06
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DB7B84-5C99-BB41-9F4A-F3DF600F7B2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF6E87CD-CED2-904E-B0C0-EB32B70B0B8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters with Distributions" sheetId="1" r:id="rId1"/>
@@ -1267,11 +1267,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I305"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="6" ySplit="20" topLeftCell="G272" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="F294" sqref="F294"/>
+      <selection pane="bottomRight" activeCell="F295" sqref="F295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7203,13 +7203,13 @@
         <v>44201</v>
       </c>
       <c r="B293" s="19">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C293" s="19">
         <v>10</v>
       </c>
       <c r="D293" s="23">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E293" s="23">
         <v>1</v>
@@ -7220,12 +7220,24 @@
       <c r="G293" s="23"/>
     </row>
     <row r="294" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A294" s="20"/>
-      <c r="B294" s="19"/>
-      <c r="C294" s="19"/>
-      <c r="D294" s="23"/>
-      <c r="E294" s="23"/>
-      <c r="F294" s="23"/>
+      <c r="A294" s="20">
+        <v>44202</v>
+      </c>
+      <c r="B294" s="19">
+        <v>241</v>
+      </c>
+      <c r="C294" s="19">
+        <v>6</v>
+      </c>
+      <c r="D294" s="23">
+        <v>58</v>
+      </c>
+      <c r="E294" s="23">
+        <v>0</v>
+      </c>
+      <c r="F294" s="23">
+        <v>203</v>
+      </c>
       <c r="G294" s="23"/>
     </row>
     <row r="295" spans="1:7" x14ac:dyDescent="0.2">
@@ -7474,8 +7486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7582,7 +7594,7 @@
         <v>37</v>
       </c>
       <c r="B8" s="3">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="C8">
         <v>1000</v>
@@ -7596,7 +7608,7 @@
         <v>85</v>
       </c>
       <c r="B9" s="3">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="C9"/>
     </row>

</xml_diff>

<commit_message>
SF data through 2021-01-07
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF6E87CD-CED2-904E-B0C0-EB32B70B0B8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1703E0DC-B127-0040-B7ED-3B568EEE6234}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters with Distributions" sheetId="1" r:id="rId1"/>
@@ -1267,11 +1267,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I305"/>
   <sheetViews>
-    <sheetView zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="20" topLeftCell="G272" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="20" topLeftCell="G277" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="F295" sqref="F295"/>
+      <selection pane="bottomRight" activeCell="F296" sqref="F296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7241,17 +7241,28 @@
       <c r="G294" s="23"/>
     </row>
     <row r="295" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A295" s="20"/>
-      <c r="B295" s="19"/>
-      <c r="C295" s="19"/>
-      <c r="D295" s="23"/>
-      <c r="E295" s="23"/>
-      <c r="F295" s="23"/>
+      <c r="A295" s="20">
+        <v>44203</v>
+      </c>
+      <c r="B295" s="19">
+        <v>242</v>
+      </c>
+      <c r="C295" s="19">
+        <v>5</v>
+      </c>
+      <c r="D295" s="23">
+        <v>60</v>
+      </c>
+      <c r="E295" s="23">
+        <v>0</v>
+      </c>
+      <c r="F295" s="23">
+        <v>205</v>
+      </c>
       <c r="G295" s="23"/>
     </row>
     <row r="296" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A296" s="20"/>
-      <c r="B296" s="19"/>
       <c r="C296" s="19"/>
       <c r="D296" s="23"/>
       <c r="E296" s="23"/>
@@ -7350,7 +7361,7 @@
       <formula1>43831</formula1>
       <formula2>44561</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I299 H63:H299 H5:H60 F133:F148 B71:B323 B5:B64 C5:C322" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I299 H63:H299 H5:H60 F133:F148 B5:B64 C5:C322 B71:B295 B297:B323" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>0</formula1>
       <formula2>10000000</formula2>
     </dataValidation>
@@ -7486,7 +7497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
SF data through 2021-01-08
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1703E0DC-B127-0040-B7ED-3B568EEE6234}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1620B84-E2D1-7141-9053-1B3C2A82AE25}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1271,7 +1271,7 @@
       <pane xSplit="6" ySplit="20" topLeftCell="G277" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="F296" sqref="F296"/>
+      <selection pane="bottomRight" activeCell="F297" sqref="F297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7262,11 +7262,24 @@
       <c r="G295" s="23"/>
     </row>
     <row r="296" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A296" s="20"/>
-      <c r="C296" s="19"/>
-      <c r="D296" s="23"/>
-      <c r="E296" s="23"/>
-      <c r="F296" s="23"/>
+      <c r="A296" s="20">
+        <v>44204</v>
+      </c>
+      <c r="B296" s="3">
+        <v>239</v>
+      </c>
+      <c r="C296" s="19">
+        <v>8</v>
+      </c>
+      <c r="D296" s="23">
+        <v>59</v>
+      </c>
+      <c r="E296" s="23">
+        <v>0</v>
+      </c>
+      <c r="F296" s="23">
+        <v>218</v>
+      </c>
       <c r="G296" s="23"/>
     </row>
     <row r="297" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
SF data through 2021-01-09
</commit_message>
<xml_diff>
--- a/Inputs/SF.xlsx
+++ b/Inputs/SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1620B84-E2D1-7141-9053-1B3C2A82AE25}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DEFB5A-A3AA-8046-82D9-FB8236EA276F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4140" yWindow="1100" windowWidth="29440" windowHeight="19500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1271,7 +1271,7 @@
       <pane xSplit="6" ySplit="20" topLeftCell="G277" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="F297" sqref="F297"/>
+      <selection pane="bottomRight" activeCell="G297" sqref="G297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7283,12 +7283,24 @@
       <c r="G296" s="23"/>
     </row>
     <row r="297" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A297" s="20"/>
-      <c r="B297" s="19"/>
-      <c r="C297" s="19"/>
-      <c r="D297" s="23"/>
-      <c r="E297" s="23"/>
-      <c r="F297" s="23"/>
+      <c r="A297" s="20">
+        <v>44205</v>
+      </c>
+      <c r="B297" s="19">
+        <v>254</v>
+      </c>
+      <c r="C297" s="19">
+        <v>11</v>
+      </c>
+      <c r="D297" s="23">
+        <v>59</v>
+      </c>
+      <c r="E297" s="23">
+        <v>0</v>
+      </c>
+      <c r="F297" s="23">
+        <v>233</v>
+      </c>
       <c r="G297" s="23"/>
     </row>
     <row r="298" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>